<commit_message>
Fixes #288 - Issue with contents of the Bewertungsbogen
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\HT\A1811_HT_Infos\A1811_Infos\Studienbetrieb\Projektschiene\Bewertung_Projekte_5_und_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midna/_repositories/aadjou/ProStudCreator/ProStudCreator/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AF440F-4127-42F7-A9A0-9B0646DBBC92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4B17EA9-88E4-3F4F-BE62-1332A70484FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="30220" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_Toc156968632" localSheetId="0">'1. Gesamtbewertung (Text)'!$A$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'2. Detailbewertung (Excel)'!$A$1:$G$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'2. Detailbewertung (Excel)'!$A$1:$G$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -182,36 +182,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Theoretische Arbeit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Praktische Arbeit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
     <t>ORGANISATION, PLANUNG, METHODIK</t>
   </si>
   <si>
@@ -344,27 +314,7 @@
     <t>Bonuspunkte: nur für grössere Herausforderungen in 3 Bereichen.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">   Bonus
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>absolute Notenkorrektur
-   festgelegt durch Betreuer</t>
-    </r>
-  </si>
-  <si>
     <t>Bonusnote (Feld C33):  Zusatznotenpunkte, gerundet auf 1/10.</t>
-  </si>
-  <si>
-    <t>Braucht es je 10 Punkte?
-Direkt in Bonusnote umrechnen?</t>
   </si>
   <si>
     <t>Eine detaillierte Kommunikation der Bewertung ist bei den P5 obligatorisch (kann auch erst zu Beginn des Folgesemesters stattfinden) und bei den P6 wünschenswert (manchmal sind die Studierenden gar nicht mehr verfügbar). Ist die Thesis im ersten Anlauf nicht bestanden, ist ein Feedback obligatorisch.</t>
@@ -410,6 +360,63 @@
   </si>
   <si>
     <t xml:space="preserve">Betreuende(r) Dozierende(r): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Bonus</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Absolute Notenkorrektur</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+   festgelegt durch Betreuer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Theoretische Arbeit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 3 ergeben.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Praktische Arbeit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 3 ergeben.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -663,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1266,13 +1273,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1657,6 +1712,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1666,9 +1745,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1705,27 +1781,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1734,12 +1789,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1790,11 +1839,36 @@
     <xf numFmtId="165" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="50" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="53" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4797,13 +4871,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4873,11 +4947,77 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Textfeld 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A77AA03E-30B5-3E44-A474-6AE3CF95E4B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5672667" y="39948556"/>
+          <a:ext cx="5023555" cy="832555"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:spcAft>
+              <a:spcPts val="200"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5202,268 +5342,262 @@
   </sheetPr>
   <dimension ref="A6:C49"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.54296875" style="128" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="124"/>
-    <col min="4" max="16384" width="10.7265625" style="82"/>
+    <col min="1" max="1" width="32.1640625" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.5" style="128" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="124"/>
+    <col min="4" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="s">
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-    </row>
-    <row r="8" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="137"/>
+      <c r="C6" s="137"/>
+    </row>
+    <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="121" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="130"/>
-      <c r="C8" s="130"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="B8" s="138"/>
+      <c r="C8" s="138"/>
+    </row>
+    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="143"/>
-      <c r="C9" s="144"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="150"/>
+      <c r="C9" s="151"/>
+    </row>
+    <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="121" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="130"/>
-      <c r="C10" s="130"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B10" s="138"/>
+      <c r="C10" s="138"/>
+    </row>
+    <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="130"/>
-      <c r="C11" s="130"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="138"/>
+      <c r="C11" s="138"/>
+    </row>
+    <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="122"/>
       <c r="B12" s="123"/>
     </row>
-    <row r="13" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+    <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="135"/>
-      <c r="C13" s="136"/>
-    </row>
-    <row r="14" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="139"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="139"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="139"/>
-    </row>
-    <row r="17" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="137"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="139"/>
-    </row>
-    <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-    </row>
-    <row r="19" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="139"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="139"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="137"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="139"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="137"/>
-      <c r="B22" s="138"/>
-      <c r="C22" s="139"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="137"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="139"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="137"/>
-      <c r="B24" s="138"/>
-      <c r="C24" s="139"/>
-    </row>
-    <row r="25" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="137"/>
-      <c r="B25" s="138"/>
-      <c r="C25" s="139"/>
-    </row>
-    <row r="26" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="137"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="139"/>
-    </row>
-    <row r="27" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="137"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="139"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="137"/>
-      <c r="B28" s="138"/>
-      <c r="C28" s="139"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="137"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="139"/>
-    </row>
-    <row r="30" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="137"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="139"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="137"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="139"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="137"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="139"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137"/>
-      <c r="B33" s="138"/>
-      <c r="C33" s="139"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="140"/>
-      <c r="B34" s="141"/>
-      <c r="C34" s="142"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="142"/>
+      <c r="C13" s="143"/>
+    </row>
+    <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="144"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="146"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="144"/>
+      <c r="B15" s="145"/>
+      <c r="C15" s="146"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="144"/>
+      <c r="B16" s="145"/>
+      <c r="C16" s="146"/>
+    </row>
+    <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="144"/>
+      <c r="B17" s="145"/>
+      <c r="C17" s="146"/>
+    </row>
+    <row r="18" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="144"/>
+      <c r="B18" s="145"/>
+      <c r="C18" s="146"/>
+    </row>
+    <row r="19" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="144"/>
+      <c r="B19" s="145"/>
+      <c r="C19" s="146"/>
+    </row>
+    <row r="20" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="144"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="146"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="144"/>
+      <c r="B21" s="145"/>
+      <c r="C21" s="146"/>
+    </row>
+    <row r="22" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="144"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="146"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="144"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="146"/>
+    </row>
+    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="144"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="146"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="144"/>
+      <c r="B25" s="145"/>
+      <c r="C25" s="146"/>
+    </row>
+    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="144"/>
+      <c r="B26" s="145"/>
+      <c r="C26" s="146"/>
+    </row>
+    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="144"/>
+      <c r="B27" s="145"/>
+      <c r="C27" s="146"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="144"/>
+      <c r="B28" s="145"/>
+      <c r="C28" s="146"/>
+    </row>
+    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="144"/>
+      <c r="B29" s="145"/>
+      <c r="C29" s="146"/>
+    </row>
+    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="144"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
+    </row>
+    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="144"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="146"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="144"/>
+      <c r="B32" s="145"/>
+      <c r="C32" s="146"/>
+    </row>
+    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="144"/>
+      <c r="B33" s="145"/>
+      <c r="C33" s="146"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="147"/>
+      <c r="B34" s="148"/>
+      <c r="C34" s="149"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="122"/>
       <c r="B35" s="123"/>
     </row>
-    <row r="36" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="130" t="s">
+    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="130"/>
+      <c r="B36" s="138"/>
       <c r="C36" s="125">
-        <f>'2. Detailbewertung (Excel)'!C34</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <f>'2. Detailbewertung (Excel)'!C35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="122"/>
       <c r="B37" s="123"/>
     </row>
-    <row r="38" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="130" t="s">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="130"/>
-      <c r="C38" s="130"/>
-    </row>
-    <row r="39" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="147" t="s">
+      <c r="B38" s="138"/>
+      <c r="C38" s="138"/>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="148"/>
-      <c r="C39" s="149"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="131" t="s">
+      <c r="B39" s="132"/>
+      <c r="C39" s="133"/>
+    </row>
+    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="131"/>
-      <c r="C40" s="131"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="139"/>
+      <c r="C40" s="139"/>
+    </row>
+    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="122"/>
       <c r="B41" s="123"/>
     </row>
-    <row r="42" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="122"/>
       <c r="B42" s="123"/>
     </row>
-    <row r="43" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="126" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="150">
+      <c r="B43" s="134">
         <f ca="1">TODAY()</f>
-        <v>43535</v>
-      </c>
-      <c r="C43" s="151"/>
-    </row>
-    <row r="44" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43655</v>
+      </c>
+      <c r="C43" s="135"/>
+    </row>
+    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="90"/>
-      <c r="B44" s="132"/>
-      <c r="C44" s="132"/>
-    </row>
-    <row r="45" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="136"/>
+      <c r="C44" s="136"/>
+    </row>
+    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="90"/>
-      <c r="B45" s="132"/>
-      <c r="C45" s="132"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="136"/>
+      <c r="C45" s="136"/>
+    </row>
+    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="127" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="132"/>
-      <c r="C46" s="132"/>
-    </row>
-    <row r="47" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="B46" s="136"/>
+      <c r="C46" s="136"/>
+    </row>
+    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="127"/>
-      <c r="B47" s="132"/>
-      <c r="C47" s="132"/>
-    </row>
-    <row r="48" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="136"/>
+      <c r="C47" s="136"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="133"/>
-      <c r="C48" s="133"/>
-    </row>
-    <row r="49" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
+    </row>
+    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="92"/>
-      <c r="B49" s="145"/>
-      <c r="C49" s="146"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A40:C40"/>
@@ -5475,6 +5609,12 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5486,26 +5626,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" style="46" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" customWidth="1"/>
-    <col min="6" max="6" width="65.81640625" customWidth="1"/>
-    <col min="7" max="7" width="66.7265625" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="6" max="6" width="65.83203125" customWidth="1"/>
+    <col min="7" max="7" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="68" customFormat="1" ht="29.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" s="68" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="71" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="70"/>
       <c r="D1" s="70"/>
@@ -5513,7 +5653,7 @@
       <c r="F1" s="70"/>
       <c r="G1" s="70"/>
     </row>
-    <row r="2" spans="1:7" s="68" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" s="68" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -5522,9 +5662,9 @@
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
     </row>
-    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="152" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="152"/>
@@ -5532,7 +5672,7 @@
       <c r="F3" s="152"/>
       <c r="G3" s="152"/>
     </row>
-    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="153" t="s">
         <v>9</v>
       </c>
@@ -5542,7 +5682,7 @@
       <c r="F4" s="154"/>
       <c r="G4" s="154"/>
     </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="12" t="s">
         <v>0</v>
@@ -5561,20 +5701,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="44" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="44" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="95">
         <v>1</v>
       </c>
-      <c r="B6" s="163" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="165"/>
+      <c r="B6" s="161" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="163"/>
       <c r="G6" s="96"/>
     </row>
-    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="48">
         <v>1.1000000000000001</v>
       </c>
@@ -5584,121 +5724,111 @@
       <c r="C7" s="113">
         <v>2</v>
       </c>
-      <c r="D7" s="110">
-        <v>4</v>
-      </c>
+      <c r="D7" s="110"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="74"/>
     </row>
-    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="48">
         <v>1.2</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="111">
         <v>1</v>
       </c>
-      <c r="D8" s="110">
-        <v>4.5</v>
-      </c>
+      <c r="D8" s="110"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="74"/>
     </row>
-    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="49">
         <v>1.3</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="112">
         <v>1</v>
       </c>
-      <c r="D9" s="110">
-        <v>4.5</v>
-      </c>
+      <c r="D9" s="110"/>
       <c r="E9" s="22"/>
       <c r="F9" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="75"/>
     </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="50"/>
       <c r="B10" s="103" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="104">
         <v>1</v>
       </c>
       <c r="D10" s="115">
         <f>(C7*D7+C8*D8+C9*D9)/SUM(C7:C9)</f>
-        <v>4.25</v>
+        <v>0</v>
       </c>
       <c r="E10" s="105"/>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="97">
         <v>2</v>
       </c>
-      <c r="B11" s="166" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="167"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="168"/>
+      <c r="B11" s="164" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="165"/>
+      <c r="D11" s="165"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="166"/>
       <c r="G11" s="98"/>
     </row>
-    <row r="12" spans="1:7" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="151.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="51">
         <v>2.1</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C12" s="113">
         <v>2</v>
       </c>
-      <c r="D12" s="110">
-        <v>4</v>
-      </c>
+      <c r="D12" s="110"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="72"/>
     </row>
-    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="49">
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C13" s="112">
         <v>1</v>
       </c>
-      <c r="D13" s="110">
-        <v>4</v>
-      </c>
+      <c r="D13" s="110"/>
       <c r="E13" s="22"/>
       <c r="F13" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="73"/>
     </row>
-    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="49">
         <v>2.2999999999999998</v>
       </c>
@@ -5708,16 +5838,14 @@
       <c r="C14" s="112">
         <v>2</v>
       </c>
-      <c r="D14" s="110">
-        <v>4</v>
-      </c>
+      <c r="D14" s="110"/>
       <c r="E14" s="22"/>
       <c r="F14" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="74"/>
     </row>
-    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="49">
         <v>2.4</v>
       </c>
@@ -5727,16 +5855,14 @@
       <c r="C15" s="112">
         <v>1</v>
       </c>
-      <c r="D15" s="110">
-        <v>4</v>
-      </c>
+      <c r="D15" s="110"/>
       <c r="E15" s="22"/>
       <c r="F15" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="75"/>
     </row>
-    <row r="16" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="65">
         <v>2.5</v>
       </c>
@@ -5746,43 +5872,41 @@
       <c r="C16" s="112">
         <v>1</v>
       </c>
-      <c r="D16" s="110">
-        <v>4</v>
-      </c>
+      <c r="D16" s="110"/>
       <c r="E16" s="42"/>
       <c r="F16" s="43"/>
       <c r="G16" s="76"/>
     </row>
-    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
       <c r="B17" s="103" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="116">
         <v>4</v>
       </c>
       <c r="D17" s="115">
         <f>(C12*D12+C13*D13+C14*D14+C15*D15+C16*D16)/SUM(C12:C16)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E17" s="105"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="1:8" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="99">
         <v>3</v>
       </c>
-      <c r="B18" s="163" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="169"/>
-      <c r="D18" s="169"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="165"/>
+      <c r="B18" s="161" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="167"/>
+      <c r="D18" s="167"/>
+      <c r="E18" s="162"/>
+      <c r="F18" s="163"/>
       <c r="G18" s="100"/>
     </row>
-    <row r="19" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="49">
         <v>3.1</v>
       </c>
@@ -5792,28 +5916,24 @@
       <c r="C19" s="112">
         <v>1</v>
       </c>
-      <c r="D19" s="110">
-        <v>6</v>
-      </c>
+      <c r="D19" s="110"/>
       <c r="E19" s="19"/>
       <c r="F19" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="74"/>
     </row>
-    <row r="20" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="49">
         <v>3.2</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="112">
         <v>1</v>
       </c>
-      <c r="D20" s="110">
-        <v>4</v>
-      </c>
+      <c r="D20" s="110"/>
       <c r="E20" s="22"/>
       <c r="F20" s="20" t="s">
         <v>23</v>
@@ -5822,7 +5942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="64">
         <v>3.3</v>
       </c>
@@ -5832,58 +5952,54 @@
       <c r="C21" s="112">
         <v>1</v>
       </c>
-      <c r="D21" s="110">
-        <v>3</v>
-      </c>
+      <c r="D21" s="110"/>
       <c r="E21" s="28"/>
       <c r="F21" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="77"/>
     </row>
-    <row r="22" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
       <c r="B22" s="103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="117">
         <v>2</v>
       </c>
       <c r="D22" s="118">
         <f>(C19*D19+C20*D20+C21*D21)/SUM(C19:C21)</f>
-        <v>4.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="101">
         <v>4</v>
       </c>
-      <c r="B23" s="163" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="169"/>
-      <c r="D23" s="169"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="165"/>
+      <c r="B23" s="161" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
       <c r="G23" s="98"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="55">
         <v>4.0999999999999996</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="109">
         <v>1</v>
       </c>
-      <c r="D24" s="110">
-        <v>4</v>
-      </c>
+      <c r="D24" s="110"/>
       <c r="E24" s="26"/>
       <c r="F24" s="20" t="s">
         <v>23</v>
@@ -5891,27 +6007,25 @@
       <c r="G24" s="75"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="168.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="53">
         <v>4.2</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="111">
         <f>2-C24</f>
         <v>1</v>
       </c>
-      <c r="D25" s="110">
-        <v>3</v>
-      </c>
+      <c r="D25" s="110"/>
       <c r="E25" s="27"/>
       <c r="F25" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="74"/>
     </row>
-    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="64">
         <v>4.3</v>
       </c>
@@ -5921,170 +6035,180 @@
       <c r="C26" s="111">
         <v>1</v>
       </c>
-      <c r="D26" s="110">
-        <v>4</v>
-      </c>
+      <c r="D26" s="110"/>
       <c r="E26" s="28"/>
       <c r="F26" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="77"/>
     </row>
-    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
       <c r="B27" s="103" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="117">
         <v>1</v>
       </c>
       <c r="D27" s="118">
         <f>(C24*D24+C25*D25+C26*D26)/SUM(C24:C26)</f>
-        <v>3.6666666666666665</v>
+        <v>0</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52"/>
       <c r="B28" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="170">
+      <c r="C28" s="168">
         <f>(C10*D10+C17*D17+C22*D22+C27*D27)/SUM(C10,C17,C22,C27)</f>
-        <v>4.0729166666666661</v>
-      </c>
-      <c r="D28" s="171"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="169"/>
       <c r="E28" s="31"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="95">
         <v>5</v>
       </c>
-      <c r="B29" s="163" t="s">
+      <c r="B29" s="161" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="165"/>
+      <c r="C29" s="162"/>
+      <c r="D29" s="162"/>
+      <c r="E29" s="162"/>
+      <c r="F29" s="163"/>
       <c r="G29" s="102"/>
     </row>
-    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="63"/>
       <c r="B30" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="159">
-        <v>5</v>
-      </c>
-      <c r="D30" s="160"/>
+      <c r="C30" s="157">
+        <v>0</v>
+      </c>
+      <c r="D30" s="158"/>
       <c r="E30" s="59"/>
       <c r="F30" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="74" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="74"/>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="63"/>
       <c r="B31" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="159">
-        <v>5</v>
-      </c>
-      <c r="D31" s="160"/>
+      <c r="C31" s="157">
+        <v>0</v>
+      </c>
+      <c r="D31" s="158"/>
       <c r="E31" s="60"/>
       <c r="F31" s="25" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="78"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="54"/>
       <c r="B32" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="161">
-        <v>5</v>
-      </c>
-      <c r="D32" s="162"/>
+        <v>56</v>
+      </c>
+      <c r="C32" s="159">
+        <v>0</v>
+      </c>
+      <c r="D32" s="160"/>
       <c r="E32" s="61"/>
       <c r="F32" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="79"/>
     </row>
-    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="57"/>
-      <c r="B33" s="108" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="155">
-        <v>0.4</v>
-      </c>
-      <c r="D33" s="156"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="157">
-        <f>ROUND(C28+C33,1)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D34" s="158"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-    </row>
-    <row r="35" spans="1:7" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="58"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="C37" s="5"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="17"/>
-      <c r="D38" s="2"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
+    <row r="33" spans="1:7" s="175" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="172"/>
+      <c r="B33" s="176" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="177">
+        <f>0.25*SUM(C30:D32)/30</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="178"/>
+      <c r="E33" s="173"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="174"/>
+    </row>
+    <row r="34" spans="1:7" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="57"/>
+      <c r="B34" s="108" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="170">
+        <v>0</v>
+      </c>
+      <c r="D34" s="171"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="56"/>
+      <c r="B35" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="155">
+        <f>ROUND(C28+C33+C34,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="156"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+    </row>
+    <row r="36" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="45"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="58"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C38" s="5"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C39" s="17"/>
+      <c r="D39" s="2"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
-    <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -6094,6 +6218,7 @@
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -6116,49 +6241,49 @@
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="115" style="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.15">
       <c r="A3" s="81" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A5" s="119" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A7" s="119" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A8" s="119" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="119" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="119" t="s">
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A10" s="119" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="119" t="s">
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A12" s="119" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A13" s="119" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="119" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="119" t="s">
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A15" s="119" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="119" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -6175,85 +6300,85 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="82" customWidth="1"/>
-    <col min="2" max="2" width="67.81640625" style="80" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="82" customWidth="1"/>
+    <col min="2" max="2" width="67.83203125" style="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.15">
       <c r="A3" s="81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="84" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
-        <v>39</v>
-      </c>
       <c r="B6" s="85" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="83"/>
     </row>
-    <row r="8" spans="1:2" ht="50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="56" x14ac:dyDescent="0.15">
       <c r="A8" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="83"/>
+    </row>
+    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="85" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-    </row>
-    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
-        <v>40</v>
-      </c>
       <c r="B10" s="87" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="13" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="88"/>
       <c r="B11" s="89"/>
     </row>
-    <row r="12" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="90"/>
       <c r="B12" s="89" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="90"/>
       <c r="B13" s="91"/>
     </row>
-    <row r="14" spans="1:2" ht="25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="90"/>
       <c r="B14" s="89" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="90"/>
       <c r="B15" s="91"/>
     </row>
-    <row r="16" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="90"/>
       <c r="B16" s="94" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="90"/>
       <c r="B17" s="91"/>
     </row>
-    <row r="18" spans="1:2" ht="50" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="92"/>
       <c r="B18" s="93" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds new version of the Bewertungsbogen
the up to date version of the Bewertungsbogen can always be found on the AD in the directory
T:\A1811_HT_Infos\A1811_Infos\Studienbetrieb\Projektschiene\Bewertung_Projekte_5_und_6

This is the version of May 22.
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\HT\A1811_HT_Infos\A1811_Infos\Studienbetrieb\Projektschiene\Bewertung_Projekte_5_und_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ProStudCreator\ProStudCreator\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AF440F-4127-42F7-A9A0-9B0646DBBC92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3105" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -22,20 +21,49 @@
     <definedName name="_Toc156968632" localSheetId="0">'1. Gesamtbewertung (Text)'!$A$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2. Detailbewertung (Excel)'!$A$1:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Samuel Vogel</author>
+  </authors>
+  <commentList>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Zusammensetzung Block 2:
+Samuel Vogel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Gew 3 Theorie/Praxis
+Gew 2 Analyse
+Gew 2 Ziel/Betreuung</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Name:</t>
   </si>
@@ -104,12 +132,12 @@
     <t>Zwischennote vor Bonus</t>
   </si>
   <si>
-    <t>Präsentationen (Zwpräs+Schlusspräs)(P5 und P6)</t>
-  </si>
-  <si>
     <t>Beurteilungsbogen für die Bachelor-Thesis</t>
   </si>
   <si>
+    <t>Student:</t>
+  </si>
+  <si>
     <t>Projekttitel:</t>
   </si>
   <si>
@@ -123,6 +151,22 @@
   </si>
   <si>
     <t>Klassifizierung der Arbeit (Zutreffendes ankreuzen):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betreuender Dozent: </t>
+  </si>
+  <si>
+    <r>
+      <t>Betreuender Dozent:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
   <si>
     <r>
@@ -167,90 +211,12 @@
     <t>Selbstständigkeit / Betreuungsintensität</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Lösungskonzept / Strategie
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Je nach Komplexität der Aufgabenstellung soll die Gewichtung zwischen 0.2 (einfach) und 1 (komplex) liegen.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Theoretische Arbeit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Praktische Arbeit
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
     <t>ORGANISATION, PLANUNG, METHODIK</t>
   </si>
   <si>
-    <t>SELBSTSTÄNDIGKEIT, ANWENDUNG VON WISSEN</t>
-  </si>
-  <si>
     <t>KOMMUNIKATION, MOTIVATION</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Zusammenarbeit und Kommunikation intern
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Intern oder Extern verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Zusammenarbeit und Kommunikation extern
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Intern oder Extern verschoben werden. Die Summe der beiden Blöcke muss immer 2 ergeben.</t>
-    </r>
-  </si>
-  <si>
     <t>DOKUMENTATION,  WISSENSTRANSFER</t>
   </si>
   <si>
@@ -275,9 +241,6 @@
     <t>Bei der Abschlussbesprechung der Arbeit wird das Blatt "1. Gesamtbewertung" an die Studierenden abgegeben.</t>
   </si>
   <si>
-    <t>Die Kommentare sind ein Hilfsmittel für die Projektbetreuer und u.U. nicht geeignet, weitergegeben zu werden. Sie dienen darum primär als Grundlage für die Notengebung und die Schlussbesprechung, aber nicht direkt für die Kommunikation der Bewertung.</t>
-  </si>
-  <si>
     <t>Lerneffekt durch die Bewertung und die Rückmeldungen.</t>
   </si>
   <si>
@@ -305,22 +268,10 @@
     <t>Blocknote 4 - Gewicht: 1</t>
   </si>
   <si>
-    <t>Die Gewichtungsfaktoren (Werte 0, 1 oder 2) im Blatt "2. Detailbewertung" werden in der Anfangsphase des Projektes festgelegt (der Aufgabenstellung angepasst) und den Studierenden abgegeben.</t>
-  </si>
-  <si>
     <t>Anleitung zum Ausfüllen der Detailbewertung</t>
   </si>
   <si>
     <t>Nur die grau unterlegten Felder ausfüllen.</t>
-  </si>
-  <si>
-    <t>Werte: 0 oder 1 oder 2</t>
-  </si>
-  <si>
-    <t>Gewichtungsfaktoren (Spalte C) ausfüllen bei der Projektvereinbarung.</t>
-  </si>
-  <si>
-    <t>Die Gewichtungen der Blocknote (z.B. Zelle C10) sind vorgegeben.</t>
   </si>
   <si>
     <r>
@@ -341,7 +292,29 @@
     <t>Diese Punkte gehen nicht in eine Rechnung ein, sie sind nur ein Hilfsmittel für den Betreuer.</t>
   </si>
   <si>
-    <t>Bonuspunkte: nur für grössere Herausforderungen in 3 Bereichen.</t>
+    <t>Bonusnote (Feld C33):  Zusatznotenpunkte, gerundet auf 1/10.</t>
+  </si>
+  <si>
+    <t>Eine detaillierte Kommunikation der Bewertung ist bei den P5 obligatorisch (kann auch erst zu Beginn des Folgesemesters stattfinden) und bei den P6 wünschenswert (manchmal sind die Studierenden gar nicht mehr verfügbar). Ist die Thesis im ersten Anlauf nicht bestanden, ist ein Feedback obligatorisch.</t>
+  </si>
+  <si>
+    <t>Verteidigung (P6)
+(Bei P5 Gewicht auf 0 setzen)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lösungskonzept / Strategie
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Gewichtung aufgrund der Komplexität des Projektes festlegen.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -356,22 +329,99 @@
         <family val="2"/>
       </rPr>
       <t>absolute Notenkorrektur
-   festgelegt durch Betreuer</t>
+   festgelegt durch Betreuer aufgrund der
+   Bonuspunkte (Wert wird nicht berechnet)</t>
     </r>
   </si>
   <si>
-    <t>Bonusnote (Feld C33):  Zusatznotenpunkte, gerundet auf 1/10.</t>
-  </si>
-  <si>
-    <t>Braucht es je 10 Punkte?
-Direkt in Bonusnote umrechnen?</t>
-  </si>
-  <si>
-    <t>Eine detaillierte Kommunikation der Bewertung ist bei den P5 obligatorisch (kann auch erst zu Beginn des Folgesemesters stattfinden) und bei den P6 wünschenswert (manchmal sind die Studierenden gar nicht mehr verfügbar). Ist die Thesis im ersten Anlauf nicht bestanden, ist ein Feedback obligatorisch.</t>
-  </si>
-  <si>
-    <t>Verteidigung (P6)
-(Bei P5 Gewicht auf 0 setzen)</t>
+    <t>Die Gewichtungen der Blocknoten (Zellen C10, C17, C22 und C27) sind vorgegeben.</t>
+  </si>
+  <si>
+    <t>Die Gewichtungsfaktoren im Blatt "2. Detailbewertung" werden in der Anfangsphase des Projektes festgelegt (der Aufgabenstellung angepasst) und den Studierenden abgegeben.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Theoretische Arbeit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Praktische Arbeit
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Theorie oder Praxis verschoben werden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zusammenarbeit und Kommunikation intern
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Intern oder Extern verschoben werden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zusammenarbeit und Kommunikation extern
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Die Gewichtung soll der Ausrichtung des Projekts entsprechend Richtung Intern oder Extern verschoben werden.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gewichtungsfaktoren (Spalte C) in der Anphangsphase des Projektes festlegen.</t>
+  </si>
+  <si>
+    <t>FACHLICHES, ANWENDUNG VON WISSEN, SELBSTÄNDIGKEIT</t>
+  </si>
+  <si>
+    <t>Präsentationen (Zwischen- und Schlusspräsentation, P5 und P6)</t>
+  </si>
+  <si>
+    <t>Bonuspunkte: nur für grössere bzw. unvorhergesehene Herausforderungen in 3 Bereichen.</t>
+  </si>
+  <si>
+    <t>Sparsam einsetzen, max. 0.2 Notenpunkte!</t>
+  </si>
+  <si>
+    <t>Mit dem Bonus keine Notenkosmetik betreiben.</t>
+  </si>
+  <si>
+    <t>Benotung im oberen Teil berücksichtigen oder mit dem Bonus.</t>
+  </si>
+  <si>
+    <t>Achtung: Bonus nicht doppelt vergeben, d.h. grössere Herausforderungen entweder bei der</t>
   </si>
   <si>
     <r>
@@ -389,39 +439,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Dieser Bewertungsbogen wird von der betreunden Person ausgefüllt. Bei zwei betreuenden Personen wird er von beiden unabhängig ausgefüllt und danach abgeglichen. Wo möglich und sinnvoll wird ein Kommentar zu jeder Bewertung verfasst. Die Studierenden erhalten in jedem Fall die Würdigung in Papierform. Falls erwünscht wird auch der Bewertungsbogen in PDF From abgegeben. Nach der Projektarbeit 5 muss dieser Bewertungsbogen zwingend mit den Studierenden besprochen und auf mögliches Verbesserungspotential für die kommende Projektarbeit 6 hingewiesen werden. Nach Abschluss der Projektarbeit 6 wird der Bewertungsbogen auf Wunsch der Studierenden mit diesen besprochen.</t>
+      <t xml:space="preserve"> Dieser Bewertungsbogen wird von der betreunden Person ausgefüllt. Bei zwei betreuenden Personen wird er von beiden unabhängig ausgefüllt und danach abgeglichen. Wo möglich und sinnvoll wird ein Kommentar zu jeder Bewertung verfasst. Die Studierenden erhalten in jedem Fall die Würdigung in Papierform. Falls erwünscht, wird auch der Bewertungsbogen in PDF-From abgegeben. Nach der Projektarbeit 5 muss dieser Bewertungsbogen zwingen mit den Studierenden besprochen und auf mögliches Verbesserungspotential für die kommende Projektarbeit 6 hingewiesen werden. Nach Abschluss der Projektarbeit 6 wird der Bewertungsbogen auf Wunsch der Studierenden mit diesen besprochen.</t>
     </r>
   </si>
   <si>
-    <t>Studierende(r):</t>
-  </si>
-  <si>
-    <r>
-      <t>Betreuende(r) Dozierende(r):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Betreuende(r) Dozierende(r): </t>
+    <t>Die Kommentare (Spalte G) sind ein Hilfsmittel für die Projektbetreuer und u.U. nicht geeignet, weitergegeben zu werden. Sie dienen darum primär als Grundlage für die Notengebung und die Schlussbesprechung, aber nicht direkt für die Kommunikation der Bewertung.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -429,7 +463,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -568,6 +601,19 @@
       <charset val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1272,7 +1318,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1284,7 +1330,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1300,100 +1346,46 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1404,113 +1396,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1552,49 +1480,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1602,75 +1488,250 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1684,7 +1745,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1699,17 +1760,38 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1720,31 +1802,42 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1763,38 +1856,38 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1834,7 +1927,7 @@
         <xdr:cNvPr id="1054" name="Picture 3" descr="FHNW_HT_10mm">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,7 +2006,7 @@
         <xdr:cNvPr id="3" name="Textfeld 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1959,7 +2052,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Innovatives Lösungskonzept übertrifft die Erwartungen klar, effektive kreative Strategie</a:t>
+            <a:t>Innovatives Lösungskonzept, übertrifft die Erwartungen klar, effektive kreative Strategie</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2103,7 +2196,7 @@
         <xdr:cNvPr id="7" name="Textfeld 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2149,7 +2242,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Abgabe Termingerecht; Überdurchschnittliche, unerwartete Analyse der</a:t>
+            <a:t>Abgabe termingerecht, überdurchschnittliche/unerwartete Analyse der</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
@@ -2161,11 +2254,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> Einzelfragen im thematischen Zusammenhang</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t> und wesentlicher eigener inhaltlicher Beitrag zur</a:t>
+            <a:t> Einzelfragen im thematischen Zusammenhang,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t> wesentlicher eigener inhaltlicher Beitrag zur</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
@@ -2194,7 +2287,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
+            <a:t>Abgabe termingerecht; </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
@@ -2227,7 +2320,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
+            <a:t>Abgabe Termingerecht, </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
@@ -2257,15 +2350,15 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Umsetzung der Aufgabenstellung nicht nur teilweise erkennbar,</a:t>
+            <a:t>Abgabe termingerecht, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Umsetzung der Aufgabenstellung nur teilweise erkennbar,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> ungenügende Analyse, unpassender Lösungsansatz</a:t>
+            <a:t> ungenügende Analyse, unpassender Lösungsatz</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -2325,7 +2418,7 @@
         <xdr:cNvPr id="8" name="Textfeld 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,11 +2464,11 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Abgabe Termingerecht; Überdurchschnittliche, detaillierte Projektplanung,</a:t>
+            <a:t>Abgabe termingerecht, überdurchschnittliche und detaillierte Projektplanung,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> Arbeitsumfang realistisch abgeschätzt und abgebildet, genügend sinnvollen und klar messbare Meilensteine </a:t>
+            <a:t> Arbeitsumfang realistisch abgeschätzt und abgebildet, genügend sinnvolle und klar messbare Meilensteine </a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -2397,15 +2490,15 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Umfängliche Projektplanung, Arbeitsumfang realitätsnah</a:t>
+            <a:t>Abgabe termingerecht, u</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>mfängliche Projektplanung, Arbeitsumfang realitätsnah</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> abgeschätzt und abgebildet, mit messbaren Meilensteinen</a:t>
+            <a:t> abgeschätzt und abgebildet, mit messabren Meilensteinen</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -2427,7 +2520,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
+            <a:t>Abgabe termingerecht, </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
@@ -2435,7 +2528,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> Arbeitsumfang weitgehend realitätsnah abgeschätzt, teilweise Messbare Meilensteine</a:t>
+            <a:t> Arbeitsumfang weitgehend realitätsnah abgeschätzt, teilweise messbare Meilensteine</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -2457,7 +2550,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Abgabe Termingerecht; </a:t>
+            <a:t>Abgabe termingerecht, </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
@@ -2525,7 +2618,7 @@
         <xdr:cNvPr id="9" name="Textfeld 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2601,7 +2694,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>Durchschnittlicher Betreuungsaufwand. Kritik und Anregungen von Betreuenden werden weitgehend umgesetzt.</a:t>
+            <a:t>Durchschnittlicher Betreuungsaufwand. Kritik und Anregungen von Betreuenden werden weitgehend umgesetzt,</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2666,7 +2759,7 @@
         <xdr:cNvPr id="10" name="Textfeld 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2712,7 +2805,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Neuartiger Lösungsansatz, der die theoretischen Grundlagen klar übertrifft, sehr gut und umfassend umgesetzt</a:t>
+            <a:t>Neuartiger Lösungsansatz, der die üblichen theoretischen Grundlagenkenntnisse von Studierenden klar übertrifft, sehr gut und umfassend umgesetzt</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2829,7 +2922,7 @@
         <xdr:cNvPr id="11" name="Textfeld 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2875,7 +2968,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Äusserst umfassender und effizienter Einsatz der verfügbaren Mittel und Verfahren; Entwicklung problemspezifischer neuer Methoden</a:t>
+            <a:t>Äusserst umfassender und effizienter Einsatz der verfügbaren Mittel und Verfahren, Entwicklung problemspezifischer neuer Methoden</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2953,7 +3046,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Keine oder falsche Verfahren angewendet. Keine oder unbrauchbare Durchführung</a:t>
+            <a:t>Keine oder falsche Verfahren angewendet, keine oder unbrauchbare Durchführung</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2991,7 +3084,7 @@
         <xdr:cNvPr id="15" name="Textfeld 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3209,7 +3302,7 @@
         <xdr:cNvPr id="16" name="Textfeld 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3363,7 +3456,7 @@
         <xdr:cNvPr id="19" name="Textfeld 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3409,8 +3502,13 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Bericht vorbildlich; inhaltlich umfassend, sprachlich und gestalterisch herausragend</a:t>
-          </a:r>
+            <a:t>Bericht nachvollziehbar,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> sehr gute Leseführung, Inhalte logisch strukturiert, sehr umfassen informativ, formal sowie sprachlich und gestalterisch herausragend</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr marL="228600" indent="-228600">
@@ -3430,18 +3528,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Bericht inhaltlich vollständig, sprachlich und gestalterisch ansprechend</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr marL="228600" indent="-228600">
-            <a:spcAft>
-              <a:spcPts val="200"/>
-            </a:spcAft>
-            <a:buFont typeface="+mj-lt"/>
-            <a:buAutoNum type="arabicPeriod" startAt="4"/>
-          </a:pPr>
+            <a:t>Bericht inhaltlich vollständig, gut nachvollziehbar,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> formal korrekt,</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:solidFill>
@@ -3452,7 +3552,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Alle wesentlichen Aspekte dokumentiert, noch gut lesbar</a:t>
+            <a:t> sprachlich und gestalterisch ansprechend</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="228600" indent="-228600">
+            <a:spcAft>
+              <a:spcPts val="200"/>
+            </a:spcAft>
+            <a:buFont typeface="+mj-lt"/>
+            <a:buAutoNum type="arabicPeriod" startAt="4"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Alle wesentlichen Aspekte dokumentiert, wenig Leseführung, inhaltlich und sprachlich mehrheitlich verständlich</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -3487,7 +3609,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Wesentliche Aspekte nicht dokumentiert, Bericht unstrukturiert, Darstellung mangelhaft</a:t>
+            <a:t>Wesentliche Aspekte nicht dokumentiert, Bericht unstrukturiert, Darstellung mangelhaft, formal ungenügend</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3525,7 +3647,7 @@
         <xdr:cNvPr id="20" name="Textfeld 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3571,7 +3693,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Alle Fragen richtig und souverän beantwortet, Frage in Kontext eingeordnet. Eine Venetzung der Fachinhalte ist klar ersichtlich</a:t>
+            <a:t>Alle Fragen richtig und souverän beantwortet, Frage in Kontext eingeordnet, eine Venetzung der Fachinhalte ist klar ersichtlich</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3614,7 +3736,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Fragen zögernd, aber im Wesentlichen korrekt beantwortet; manchmal Probleme bei spezifischen Details</a:t>
+            <a:t>Fragen zögernd, aber im Wesentlichen korrekt beantwortet, manchmal Probleme bei spezifischen Details</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -3684,7 +3806,7 @@
         <xdr:cNvPr id="21" name="Textfeld 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3730,7 +3852,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Inhaltlich vollständiger, logisch aufgebauter Vortrag; grafisch sehr gut gestaltet und souverän vorgetragen; Fragen korrekt und umfassend beantwortet</a:t>
+            <a:t>Inhaltlich vollständiger und logisch aufgebauter Vortrag,  grafisch sehr gut gestaltet (unterstützend) und souverän vorgetragen, Fragen korrekt und umfassend beantwortet</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3773,7 +3895,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Vortrag inhaltlich vollständig, Einschränkungen in Aufbau und Präsentation, Fragen gut beantwortet</a:t>
+            <a:t>Im Vortrag relevante Inhalte behandelt, Einschränkungen in Aufbau (inkl. Folien) und Präsentationstechnik, Fragen gut beantwortet</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -3800,7 +3922,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Vortrag inhaltlich unzureichend, Präsentation mangelhaft; Fragen nicht oder kaum beantwortet</a:t>
+            <a:t>Vortrag inhaltlich unzureichend, Präsentation mangelhaft, Fragen nicht oder kaum beantwortet</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3838,7 +3960,7 @@
         <xdr:cNvPr id="22" name="Textfeld 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3928,7 +4050,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> das Führen eines Sitzungsprotokolls mit Dokumentation der wichtigen Beschlüsse, das kommentierte Nachbessern von Zeitplänen, sowie die Aktivierung von internem Wissen. Der/die Studierende setzte dies in folgendem Masse um:</a:t>
+            <a:t> das Führen eines Sitzungsprotokolls mit Dokumentation der wichtigen Beschlüsse, das kommentierte Nachbessern von Zeitplänen sowie die Aktivierung von internem Wissen. Der/die Studierende setzte dies in folgendem Masse um:</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -3950,7 +4072,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Äusserst</a:t>
+            <a:t>Äusserts</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
@@ -4063,7 +4185,7 @@
         <xdr:cNvPr id="23" name="Textfeld 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4129,7 +4251,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> das Führen eines Sitzungsprotokolls mit Dokumentation der wichtigen Beschlüsse, das kommentierte Nachbessern von Zeitplänen, sowie die Aktivierung von internem Wissen. Der/die Studierende setzte dies in folgendem Masse um:</a:t>
+            <a:t> das Führen eines Sitzungsprotokolls mit Dokumentation der wichtigen Beschlüsse, das kommentierte Nachbessern von Zeitplänen sowie die Aktivierung von internem Wissen. Der/die Studierende setzte dies in folgendem Masse um:</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -4151,7 +4273,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Äusserst</a:t>
+            <a:t>Äusserts</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
@@ -4264,7 +4386,7 @@
         <xdr:cNvPr id="24" name="Textfeld 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4418,7 +4540,7 @@
         <xdr:cNvPr id="25" name="Textfeld 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4557,7 +4679,7 @@
         <xdr:cNvPr id="27" name="Textfeld 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4684,7 +4806,7 @@
         <xdr:cNvPr id="28" name="Textfeld 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4811,7 +4933,7 @@
         <xdr:cNvPr id="2" name="Textfeld 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4877,7 +4999,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4952,23 +5074,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5004,23 +5109,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5196,285 +5284,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A6:C49"/>
+  <dimension ref="A6:C51"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.54296875" style="128" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="124"/>
-    <col min="4" max="16384" width="10.7265625" style="82"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="80" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="s">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-    </row>
-    <row r="8" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="130"/>
-      <c r="C8" s="130"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="121" t="s">
+      <c r="B8" s="157"/>
+      <c r="C8" s="157"/>
+    </row>
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="143"/>
-      <c r="C9" s="144"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="130"/>
-      <c r="C10" s="130"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="121" t="s">
+      <c r="B9" s="158"/>
+      <c r="C9" s="159"/>
+    </row>
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="161"/>
+    </row>
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="157"/>
+      <c r="C11" s="157"/>
+    </row>
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="130"/>
-      <c r="C11" s="130"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
-      <c r="B12" s="123"/>
-    </row>
-    <row r="13" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+      <c r="B12" s="157"/>
+      <c r="C12" s="157"/>
+    </row>
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="135"/>
-      <c r="C13" s="136"/>
-    </row>
-    <row r="14" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="139"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="139"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="139"/>
-    </row>
-    <row r="17" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="137"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="139"/>
-    </row>
-    <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-    </row>
-    <row r="19" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="139"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="139"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="137"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="139"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="137"/>
-      <c r="B22" s="138"/>
-      <c r="C22" s="139"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="137"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="139"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="137"/>
-      <c r="B24" s="138"/>
-      <c r="C24" s="139"/>
-    </row>
-    <row r="25" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="137"/>
-      <c r="B25" s="138"/>
-      <c r="C25" s="139"/>
-    </row>
-    <row r="26" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="137"/>
-      <c r="B26" s="138"/>
-      <c r="C26" s="139"/>
-    </row>
-    <row r="27" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="137"/>
-      <c r="B27" s="138"/>
-      <c r="C27" s="139"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="137"/>
-      <c r="B28" s="138"/>
-      <c r="C28" s="139"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="137"/>
-      <c r="B29" s="138"/>
-      <c r="C29" s="139"/>
-    </row>
-    <row r="30" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="137"/>
-      <c r="B30" s="138"/>
-      <c r="C30" s="139"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="137"/>
-      <c r="B31" s="138"/>
-      <c r="C31" s="139"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="137"/>
-      <c r="B32" s="138"/>
-      <c r="C32" s="139"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137"/>
-      <c r="B33" s="138"/>
-      <c r="C33" s="139"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="140"/>
-      <c r="B34" s="141"/>
-      <c r="C34" s="142"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="122"/>
-      <c r="B35" s="123"/>
-    </row>
-    <row r="36" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="130" t="s">
+      <c r="B14" s="148"/>
+      <c r="C14" s="149"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="150"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="152"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="150"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="152"/>
+    </row>
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="150"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="152"/>
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="150"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152"/>
+    </row>
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="150"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="152"/>
+    </row>
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="150"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="152"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="150"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="152"/>
+    </row>
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="150"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="152"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="150"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="152"/>
+    </row>
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="150"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="152"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="150"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="152"/>
+    </row>
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="150"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="152"/>
+    </row>
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="150"/>
+      <c r="B27" s="151"/>
+      <c r="C27" s="152"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="150"/>
+      <c r="B28" s="151"/>
+      <c r="C28" s="152"/>
+    </row>
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="150"/>
+      <c r="B29" s="151"/>
+      <c r="C29" s="152"/>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="150"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="152"/>
+    </row>
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="150"/>
+      <c r="B31" s="151"/>
+      <c r="C31" s="152"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="150"/>
+      <c r="B32" s="151"/>
+      <c r="C32" s="152"/>
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="150"/>
+      <c r="B33" s="151"/>
+      <c r="C33" s="152"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="150"/>
+      <c r="B34" s="151"/>
+      <c r="C34" s="152"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="153"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="155"/>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
+    </row>
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="130"/>
-      <c r="C36" s="125">
+      <c r="B37" s="156"/>
+      <c r="C37" s="31">
         <f>'2. Detailbewertung (Excel)'!C34</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="122"/>
-      <c r="B37" s="123"/>
-    </row>
-    <row r="38" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="130" t="s">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="24"/>
+      <c r="B38" s="25"/>
+    </row>
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="156" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="130"/>
-      <c r="C38" s="130"/>
-    </row>
-    <row r="39" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="147" t="s">
+      <c r="B39" s="156"/>
+      <c r="C39" s="156"/>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="167" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="168"/>
+      <c r="C40" s="169"/>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="170"/>
+      <c r="B41" s="171"/>
+      <c r="C41" s="172"/>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="162" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="148"/>
-      <c r="C39" s="149"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="131" t="s">
+      <c r="B42" s="162"/>
+      <c r="C42" s="162"/>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="173">
+        <f ca="1">TODAY()</f>
+        <v>43655</v>
+      </c>
+      <c r="C45" s="174"/>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="27"/>
+      <c r="B46" s="163"/>
+      <c r="C46" s="163"/>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="27"/>
+      <c r="B47" s="163"/>
+      <c r="C47" s="163"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="131"/>
-      <c r="C40" s="131"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="122"/>
-      <c r="B41" s="123"/>
-    </row>
-    <row r="42" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="122"/>
-      <c r="B42" s="123"/>
-    </row>
-    <row r="43" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="126" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="150">
-        <f ca="1">TODAY()</f>
-        <v>43535</v>
-      </c>
-      <c r="C43" s="151"/>
-    </row>
-    <row r="44" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="90"/>
-      <c r="B44" s="132"/>
-      <c r="C44" s="132"/>
-    </row>
-    <row r="45" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="90"/>
-      <c r="B45" s="132"/>
-      <c r="C45" s="132"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="127" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="132"/>
-      <c r="C46" s="132"/>
-    </row>
-    <row r="47" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="127"/>
-      <c r="B47" s="132"/>
-      <c r="C47" s="132"/>
-    </row>
-    <row r="48" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="127" t="s">
+      <c r="B48" s="163"/>
+      <c r="C48" s="163"/>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="28"/>
+      <c r="B49" s="163"/>
+      <c r="C49" s="163"/>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="133"/>
-      <c r="C48" s="133"/>
-    </row>
-    <row r="49" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="92"/>
-      <c r="B49" s="145"/>
-      <c r="C49" s="146"/>
+      <c r="B50" s="164"/>
+      <c r="C50" s="164"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="29"/>
+      <c r="B51" s="165"/>
+      <c r="C51" s="166"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A40:C41"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A40:C40"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A13:C34"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5485,601 +5579,603 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="46" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.81640625" customWidth="1"/>
-    <col min="6" max="6" width="65.81640625" customWidth="1"/>
-    <col min="7" max="7" width="66.7265625" customWidth="1"/>
+    <col min="1" max="1" width="5" style="34" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" customWidth="1"/>
+    <col min="7" max="7" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="68" customFormat="1" ht="29.5" x14ac:dyDescent="0.5">
-      <c r="B1" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-    </row>
-    <row r="2" spans="1:7" s="68" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-    </row>
-    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="152" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-    </row>
-    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="153" t="s">
+    <row r="1" spans="1:7" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A1" s="65"/>
+      <c r="B1" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+    </row>
+    <row r="2" spans="1:7" s="37" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+    </row>
+    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="69"/>
+      <c r="B3" s="175" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+    </row>
+    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="69"/>
+      <c r="B4" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-    </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
-      <c r="B5" s="12" t="s">
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+    </row>
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="70"/>
+      <c r="B5" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="66" t="s">
+      <c r="E5" s="74"/>
+      <c r="F5" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="66" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="44" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="95">
+      <c r="G5" s="75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="76">
         <v>1</v>
       </c>
-      <c r="B6" s="163" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="165"/>
-      <c r="G6" s="96"/>
-    </row>
-    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48">
+      <c r="B6" s="186" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="187"/>
+      <c r="D6" s="187"/>
+      <c r="E6" s="187"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="77"/>
+    </row>
+    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="78">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="63">
+        <v>2</v>
+      </c>
+      <c r="D7" s="62">
+        <v>4</v>
+      </c>
+      <c r="E7" s="80"/>
+      <c r="F7" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="82">
+        <v>1.2</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="61">
+        <v>1</v>
+      </c>
+      <c r="D8" s="62">
+        <v>4</v>
+      </c>
+      <c r="E8" s="80"/>
+      <c r="F8" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="85">
+        <v>1.3</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="63">
+        <v>1</v>
+      </c>
+      <c r="D9" s="62">
+        <v>4</v>
+      </c>
+      <c r="E9" s="88"/>
+      <c r="F9" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="89"/>
+      <c r="B10" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="91">
+        <v>1</v>
+      </c>
+      <c r="D10" s="92">
+        <f>(C7*D7+C8*D8+C9*D9)/SUM(C7:C9)</f>
+        <v>4</v>
+      </c>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="95">
+        <v>2</v>
+      </c>
+      <c r="B11" s="189" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="190"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="190"/>
+      <c r="F11" s="191"/>
+      <c r="G11" s="96"/>
+    </row>
+    <row r="12" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="97">
+        <v>2.1</v>
+      </c>
+      <c r="B12" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="63">
+        <v>2</v>
+      </c>
+      <c r="D12" s="62">
+        <v>4</v>
+      </c>
+      <c r="E12" s="80"/>
+      <c r="F12" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="85">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B13" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="87">
+        <v>1</v>
+      </c>
+      <c r="D13" s="62">
+        <v>4</v>
+      </c>
+      <c r="E13" s="88"/>
+      <c r="F13" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="85">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="113">
+      <c r="C14" s="87">
         <v>2</v>
       </c>
-      <c r="D7" s="110">
+      <c r="D14" s="62">
         <v>4</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="74"/>
-    </row>
-    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48">
-        <v>1.2</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="111">
+      <c r="E14" s="88"/>
+      <c r="F14" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="85">
+        <v>2.4</v>
+      </c>
+      <c r="B15" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="87">
         <v>1</v>
       </c>
-      <c r="D8" s="110">
-        <v>4.5</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="74"/>
-    </row>
-    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
-        <v>1.3</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="112">
+      <c r="D15" s="62">
+        <v>4</v>
+      </c>
+      <c r="E15" s="88"/>
+      <c r="F15" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="99">
+        <v>2.5</v>
+      </c>
+      <c r="B16" s="100" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="87">
         <v>1</v>
       </c>
-      <c r="D9" s="110">
-        <v>4.5</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="75"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="103" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="104">
-        <v>1</v>
-      </c>
-      <c r="D10" s="115">
-        <f>(C7*D7+C8*D8+C9*D9)/SUM(C7:C9)</f>
-        <v>4.25</v>
-      </c>
-      <c r="E10" s="105"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="97">
-        <v>2</v>
-      </c>
-      <c r="B11" s="166" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="167"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="98"/>
-    </row>
-    <row r="12" spans="1:7" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51">
-        <v>2.1</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="113">
-        <v>2</v>
-      </c>
-      <c r="D12" s="110">
+      <c r="D16" s="62">
         <v>4</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="72"/>
-    </row>
-    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="112">
-        <v>1</v>
-      </c>
-      <c r="D13" s="110">
+      <c r="E16" s="101"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="42"/>
+    </row>
+    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="103"/>
+      <c r="B17" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="104">
         <v>4</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="73"/>
-    </row>
-    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="112">
-        <v>2</v>
-      </c>
-      <c r="D14" s="110">
-        <v>4</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="74"/>
-    </row>
-    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
-        <v>2.4</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="112">
-        <v>1</v>
-      </c>
-      <c r="D15" s="110">
-        <v>4</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="75"/>
-    </row>
-    <row r="16" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="112">
-        <v>1</v>
-      </c>
-      <c r="D16" s="110">
-        <v>4</v>
-      </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="76"/>
-    </row>
-    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="54"/>
-      <c r="B17" s="103" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="116">
-        <v>4</v>
-      </c>
-      <c r="D17" s="115">
+      <c r="D17" s="92">
         <f>(C12*D12+C13*D13+C14*D14+C15*D15+C16*D16)/SUM(C12:C16)</f>
         <v>4</v>
       </c>
-      <c r="E17" s="105"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" spans="1:8" s="46" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="99">
+      <c r="E17" s="93"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+    </row>
+    <row r="18" spans="1:8" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="105">
         <v>3</v>
       </c>
-      <c r="B18" s="163" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="169"/>
-      <c r="D18" s="169"/>
-      <c r="E18" s="164"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="100"/>
-    </row>
-    <row r="19" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49">
+      <c r="B18" s="186" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="192"/>
+      <c r="D18" s="192"/>
+      <c r="E18" s="187"/>
+      <c r="F18" s="188"/>
+      <c r="G18" s="106"/>
+    </row>
+    <row r="19" spans="1:8" s="19" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="85">
         <v>3.1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="112">
+      <c r="C19" s="87">
         <v>1</v>
       </c>
-      <c r="D19" s="110">
-        <v>6</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="74"/>
-    </row>
-    <row r="20" spans="1:8" ht="140.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49">
+      <c r="D19" s="62">
+        <v>4</v>
+      </c>
+      <c r="E19" s="80"/>
+      <c r="F19" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" s="20" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="107">
         <v>3.2</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="112">
+      <c r="B20" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="87">
         <v>1</v>
       </c>
-      <c r="D20" s="110">
+      <c r="D20" s="62">
         <v>4</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="64">
+      <c r="E20" s="88"/>
+      <c r="F20" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="108">
         <v>3.3</v>
       </c>
-      <c r="B21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="112">
+      <c r="B21" s="109" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="87">
         <v>1</v>
       </c>
-      <c r="D21" s="110">
-        <v>3</v>
-      </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="77"/>
-    </row>
-    <row r="22" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="54"/>
-      <c r="B22" s="103" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="117">
+      <c r="D21" s="62">
+        <v>4</v>
+      </c>
+      <c r="E21" s="110"/>
+      <c r="F21" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="43"/>
+    </row>
+    <row r="22" spans="1:8" s="13" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="111"/>
+      <c r="B22" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="112">
         <v>2</v>
       </c>
-      <c r="D22" s="118">
+      <c r="D22" s="113">
         <f>(C19*D19+C20*D20+C21*D21)/SUM(C19:C21)</f>
-        <v>4.333333333333333</v>
-      </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="101">
         <v>4</v>
       </c>
-      <c r="B23" s="163" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="169"/>
-      <c r="D23" s="169"/>
-      <c r="E23" s="164"/>
-      <c r="F23" s="165"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="55">
+      <c r="E22" s="114"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="116">
+        <v>4</v>
+      </c>
+      <c r="B23" s="186" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="192"/>
+      <c r="D23" s="192"/>
+      <c r="E23" s="187"/>
+      <c r="F23" s="188"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="117">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="109">
+      <c r="B24" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="61">
         <v>1</v>
       </c>
-      <c r="D24" s="110">
+      <c r="D24" s="62">
         <v>4</v>
       </c>
-      <c r="E24" s="26"/>
-      <c r="F24" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="75"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:8" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53">
+      <c r="E24" s="118"/>
+      <c r="F24" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="41"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="1:8" s="13" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="119">
         <v>4.2</v>
       </c>
-      <c r="B25" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="111">
+      <c r="B25" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="84">
         <f>2-C24</f>
         <v>1</v>
       </c>
-      <c r="D25" s="110">
-        <v>3</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="74"/>
-    </row>
-    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64">
+      <c r="D25" s="62">
+        <v>4</v>
+      </c>
+      <c r="E25" s="120"/>
+      <c r="F25" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="40"/>
+    </row>
+    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="108">
         <v>4.3</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="111">
+      <c r="C26" s="84">
         <v>1</v>
       </c>
-      <c r="D26" s="110">
+      <c r="D26" s="62">
         <v>4</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="77"/>
-    </row>
-    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="54"/>
-      <c r="B27" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="117">
+      <c r="E26" s="110"/>
+      <c r="F26" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="43"/>
+    </row>
+    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="103"/>
+      <c r="B27" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="112">
         <v>1</v>
       </c>
-      <c r="D27" s="118">
+      <c r="D27" s="113">
         <f>(C24*D24+C25*D25+C26*D26)/SUM(C24:C26)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
-      <c r="B28" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="122"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="123"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="124"/>
+      <c r="B28" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="170">
+      <c r="C28" s="193">
         <f>(C10*D10+C17*D17+C22*D22+C27*D27)/SUM(C10,C17,C22,C27)</f>
-        <v>4.0729166666666661</v>
-      </c>
-      <c r="D28" s="171"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="95">
+        <v>4</v>
+      </c>
+      <c r="D28" s="194"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="127"/>
+      <c r="G28" s="127"/>
+    </row>
+    <row r="29" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="76">
         <v>5</v>
       </c>
-      <c r="B29" s="163" t="s">
+      <c r="B29" s="186" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="164"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="164"/>
-      <c r="F29" s="165"/>
-      <c r="G29" s="102"/>
-    </row>
-    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
-      <c r="B30" s="62" t="s">
+      <c r="C29" s="187"/>
+      <c r="D29" s="187"/>
+      <c r="E29" s="187"/>
+      <c r="F29" s="188"/>
+      <c r="G29" s="128"/>
+    </row>
+    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="129"/>
+      <c r="B30" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="159">
+      <c r="C30" s="182">
         <v>5</v>
       </c>
-      <c r="D30" s="160"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="74" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="63"/>
-      <c r="B31" s="62" t="s">
+      <c r="D30" s="183"/>
+      <c r="E30" s="131"/>
+      <c r="F30" s="132" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="40"/>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="129"/>
+      <c r="B31" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="159">
+      <c r="C31" s="182">
+        <v>0</v>
+      </c>
+      <c r="D31" s="183"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="132" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="44"/>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="111"/>
+      <c r="B32" s="134" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="184">
         <v>5</v>
       </c>
-      <c r="D31" s="160"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="78"/>
-    </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="54"/>
-      <c r="B32" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="161">
-        <v>5</v>
-      </c>
-      <c r="D32" s="162"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="79"/>
-    </row>
-    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="57"/>
-      <c r="B33" s="108" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="155">
-        <v>0.4</v>
-      </c>
-      <c r="D33" s="156"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="157">
+      <c r="D32" s="185"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="136" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="45"/>
+    </row>
+    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="137"/>
+      <c r="B33" s="138" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="178">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="179"/>
+      <c r="E33" s="139"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="140"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="141"/>
+      <c r="B34" s="142" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="180">
         <f>ROUND(C28+C33,1)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D34" s="158"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-    </row>
-    <row r="35" spans="1:7" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+        <v>4.2</v>
+      </c>
+      <c r="D34" s="181"/>
+      <c r="E34" s="143"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="33"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="58"/>
+    <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="35"/>
       <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C37" s="5"/>
-      <c r="D37" s="14"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="17"/>
+    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="18"/>
       <c r="D38" s="2"/>
       <c r="E38"/>
       <c r="F38"/>
       <c r="G38"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -6101,64 +6197,77 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CBewertungsbogen Pro5/Pro6, Seite &amp;P von 2</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="D10 D22 D17" formulaRange="1"/>
-  </ignoredErrors>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:A15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="115" style="82" customWidth="1"/>
+    <col min="1" max="1" width="115" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="119" t="s">
+    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="119" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="119" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="119" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="119" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="17.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="119" t="s">
-        <v>62</v>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="146" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="146" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="146" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="64" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -6168,92 +6277,92 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="82" customWidth="1"/>
-    <col min="2" max="2" width="67.81640625" style="80" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="23" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+    </row>
+    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="54"/>
+      <c r="B11" s="55"/>
+    </row>
+    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="56"/>
+      <c r="B12" s="55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="56"/>
+      <c r="B13" s="57"/>
+    </row>
+    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="56"/>
+      <c r="B14" s="55" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="85" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-    </row>
-    <row r="8" spans="1:2" ht="50" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="85" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-    </row>
-    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="56"/>
+      <c r="B15" s="57"/>
+    </row>
+    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="56"/>
+      <c r="B16" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="87" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="13" x14ac:dyDescent="0.25">
-      <c r="A11" s="88"/>
-      <c r="B11" s="89"/>
-    </row>
-    <row r="12" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="90"/>
-      <c r="B12" s="89" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="90"/>
-      <c r="B13" s="91"/>
-    </row>
-    <row r="14" spans="1:2" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="90"/>
-      <c r="B14" s="89" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="90"/>
-      <c r="B15" s="91"/>
-    </row>
-    <row r="16" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="90"/>
-      <c r="B16" s="94" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="90"/>
-      <c r="B17" s="91"/>
-    </row>
-    <row r="18" spans="1:2" ht="50" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
-      <c r="B18" s="93" t="s">
-        <v>42</v>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="56"/>
+      <c r="B17" s="57"/>
+    </row>
+    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="58"/>
+      <c r="B18" s="59" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed workbook protection from Bewertungsbogen
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ProStudCreator\ProStudCreator\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA08397-D528-422D-92C5-BE605DFD560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -21,17 +22,28 @@
     <definedName name="_Toc156968632" localSheetId="0">'1. Gesamtbewertung (Text)'!$A$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2. Detailbewertung (Excel)'!$A$1:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Vogel</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -449,11 +461,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -1315,7 +1327,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="195">
@@ -1343,17 +1355,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1363,7 +1375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1484,7 +1496,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1572,7 +1584,7 @@
     <xf numFmtId="1" fontId="16" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1635,7 +1647,7 @@
     <xf numFmtId="1" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1733,6 +1745,48 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1761,9 +1815,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1778,45 +1829,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1826,18 +1838,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1877,10 +1889,10 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1927,7 +1939,7 @@
         <xdr:cNvPr id="1054" name="Picture 3" descr="FHNW_HT_10mm">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,7 +2018,7 @@
         <xdr:cNvPr id="3" name="Textfeld 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2196,7 +2208,7 @@
         <xdr:cNvPr id="7" name="Textfeld 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2418,7 +2430,7 @@
         <xdr:cNvPr id="8" name="Textfeld 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2618,7 +2630,7 @@
         <xdr:cNvPr id="9" name="Textfeld 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2759,7 +2771,7 @@
         <xdr:cNvPr id="10" name="Textfeld 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2922,7 +2934,7 @@
         <xdr:cNvPr id="11" name="Textfeld 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3084,7 +3096,7 @@
         <xdr:cNvPr id="15" name="Textfeld 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3302,7 +3314,7 @@
         <xdr:cNvPr id="16" name="Textfeld 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,7 +3468,7 @@
         <xdr:cNvPr id="19" name="Textfeld 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3647,7 +3659,7 @@
         <xdr:cNvPr id="20" name="Textfeld 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3806,7 +3818,7 @@
         <xdr:cNvPr id="21" name="Textfeld 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3960,7 +3972,7 @@
         <xdr:cNvPr id="22" name="Textfeld 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4185,7 +4197,7 @@
         <xdr:cNvPr id="23" name="Textfeld 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4386,7 +4398,7 @@
         <xdr:cNvPr id="24" name="Textfeld 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4540,7 +4552,7 @@
         <xdr:cNvPr id="25" name="Textfeld 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4679,7 +4691,7 @@
         <xdr:cNvPr id="27" name="Textfeld 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4806,7 +4818,7 @@
         <xdr:cNvPr id="28" name="Textfeld 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4933,7 +4945,7 @@
         <xdr:cNvPr id="2" name="Textfeld 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5074,6 +5086,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5109,6 +5138,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5284,7 +5330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5294,265 +5340,271 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.265625" customWidth="1"/>
     <col min="2" max="2" width="80" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2"/>
+    <col min="3" max="3" width="10.73046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="157"/>
-      <c r="C8" s="157"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="170"/>
+      <c r="C8" s="170"/>
+    </row>
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="158"/>
-      <c r="C9" s="159"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="171"/>
+      <c r="C9" s="172"/>
+    </row>
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="30"/>
-      <c r="B10" s="160"/>
-      <c r="C10" s="161"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="173"/>
+      <c r="C10" s="174"/>
+    </row>
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="157"/>
-      <c r="C11" s="157"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="170"/>
+      <c r="C11" s="170"/>
+    </row>
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="157"/>
-      <c r="C12" s="157"/>
-    </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="170"/>
+      <c r="C12" s="170"/>
+    </row>
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="147" t="s">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="148"/>
-      <c r="C14" s="149"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="150"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="152"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="150"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="152"/>
-    </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="150"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="152"/>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="150"/>
-      <c r="B18" s="151"/>
-      <c r="C18" s="152"/>
-    </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="150"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="152"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="150"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="152"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="150"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="152"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="152"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="150"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="152"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="150"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="152"/>
-    </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="150"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="152"/>
-    </row>
-    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="150"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="152"/>
-    </row>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="150"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="152"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="150"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="152"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="150"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="152"/>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="150"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="150"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="152"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="150"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="152"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="150"/>
-      <c r="B33" s="151"/>
-      <c r="C33" s="152"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="150"/>
-      <c r="B34" s="151"/>
-      <c r="C34" s="152"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="153"/>
-      <c r="B35" s="154"/>
-      <c r="C35" s="155"/>
-    </row>
-    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="162"/>
+      <c r="C14" s="163"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="164"/>
+      <c r="B15" s="165"/>
+      <c r="C15" s="166"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="164"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="166"/>
+    </row>
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="164"/>
+      <c r="B17" s="165"/>
+      <c r="C17" s="166"/>
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="164"/>
+      <c r="B18" s="165"/>
+      <c r="C18" s="166"/>
+    </row>
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="164"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="166"/>
+    </row>
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="164"/>
+      <c r="B20" s="165"/>
+      <c r="C20" s="166"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="164"/>
+      <c r="B21" s="165"/>
+      <c r="C21" s="166"/>
+    </row>
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="164"/>
+      <c r="B22" s="165"/>
+      <c r="C22" s="166"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="164"/>
+      <c r="B23" s="165"/>
+      <c r="C23" s="166"/>
+    </row>
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="164"/>
+      <c r="B24" s="165"/>
+      <c r="C24" s="166"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="164"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="166"/>
+    </row>
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="164"/>
+      <c r="B26" s="165"/>
+      <c r="C26" s="166"/>
+    </row>
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="164"/>
+      <c r="B27" s="165"/>
+      <c r="C27" s="166"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="164"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+    </row>
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="164"/>
+      <c r="B29" s="165"/>
+      <c r="C29" s="166"/>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="164"/>
+      <c r="B30" s="165"/>
+      <c r="C30" s="166"/>
+    </row>
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="164"/>
+      <c r="B31" s="165"/>
+      <c r="C31" s="166"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="164"/>
+      <c r="B32" s="165"/>
+      <c r="C32" s="166"/>
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="164"/>
+      <c r="B33" s="165"/>
+      <c r="C33" s="166"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="164"/>
+      <c r="B34" s="165"/>
+      <c r="C34" s="166"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="167"/>
+      <c r="B35" s="168"/>
+      <c r="C35" s="169"/>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="24"/>
       <c r="B36" s="25"/>
     </row>
-    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="156" t="s">
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="156"/>
+      <c r="B37" s="147"/>
       <c r="C37" s="31">
         <f>'2. Detailbewertung (Excel)'!C34</f>
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="24"/>
       <c r="B38" s="25"/>
     </row>
-    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="156" t="s">
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="156"/>
-      <c r="C39" s="156"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="167" t="s">
+      <c r="B39" s="147"/>
+      <c r="C39" s="147"/>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="168"/>
-      <c r="C40" s="169"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="170"/>
-      <c r="B41" s="171"/>
-      <c r="C41" s="172"/>
-    </row>
-    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="162" t="s">
+      <c r="B40" s="154"/>
+      <c r="C40" s="155"/>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="156"/>
+      <c r="B41" s="157"/>
+      <c r="C41" s="158"/>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="162"/>
-      <c r="C42" s="162"/>
-    </row>
-    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="148"/>
+      <c r="C42" s="148"/>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="24"/>
       <c r="B43" s="25"/>
     </row>
-    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="24"/>
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="173">
+      <c r="B45" s="159">
         <f ca="1">TODAY()</f>
-        <v>43655</v>
-      </c>
-      <c r="C45" s="174"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>44459</v>
+      </c>
+      <c r="C45" s="160"/>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="27"/>
-      <c r="B46" s="163"/>
-      <c r="C46" s="163"/>
-    </row>
-    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="149"/>
+      <c r="C46" s="149"/>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="27"/>
-      <c r="B47" s="163"/>
-      <c r="C47" s="163"/>
-    </row>
-    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="149"/>
+      <c r="C47" s="149"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="163"/>
-      <c r="C48" s="163"/>
-    </row>
-    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="149"/>
+      <c r="C48" s="149"/>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="28"/>
-      <c r="B49" s="163"/>
-      <c r="C49" s="163"/>
-    </row>
-    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="149"/>
+      <c r="C49" s="149"/>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="164"/>
-      <c r="C50" s="164"/>
-    </row>
-    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="150"/>
+      <c r="C50" s="150"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="29"/>
-      <c r="B51" s="165"/>
-      <c r="C51" s="166"/>
+      <c r="B51" s="151"/>
+      <c r="C51" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
@@ -5563,12 +5615,6 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A14:C35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5579,25 +5625,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="34" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" customWidth="1"/>
-    <col min="7" max="7" width="66.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.86328125" customWidth="1"/>
+    <col min="6" max="6" width="65.86328125" customWidth="1"/>
+    <col min="7" max="7" width="66.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="37" customFormat="1" ht="29.65" x14ac:dyDescent="0.65">
       <c r="A1" s="65"/>
       <c r="B1" s="66" t="s">
         <v>32</v>
@@ -5608,7 +5654,7 @@
       <c r="F1" s="67"/>
       <c r="G1" s="67"/>
     </row>
-    <row r="2" spans="1:7" s="37" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="37" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -5617,7 +5663,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="69"/>
       <c r="B3" s="175" t="s">
         <v>70</v>
@@ -5628,7 +5674,7 @@
       <c r="F3" s="175"/>
       <c r="G3" s="175"/>
     </row>
-    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="69"/>
       <c r="B4" s="176" t="s">
         <v>9</v>
@@ -5639,7 +5685,7 @@
       <c r="F4" s="177"/>
       <c r="G4" s="177"/>
     </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="70"/>
       <c r="B5" s="71" t="s">
         <v>0</v>
@@ -5658,7 +5704,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="76">
         <v>1</v>
       </c>
@@ -5671,7 +5717,7 @@
       <c r="F6" s="188"/>
       <c r="G6" s="77"/>
     </row>
-    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78">
         <v>1.1000000000000001</v>
       </c>
@@ -5690,7 +5736,7 @@
       </c>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="82">
         <v>1.2</v>
       </c>
@@ -5709,7 +5755,7 @@
       </c>
       <c r="G8" s="40"/>
     </row>
-    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="85">
         <v>1.3</v>
       </c>
@@ -5728,7 +5774,7 @@
       </c>
       <c r="G9" s="41"/>
     </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="89"/>
       <c r="B10" s="90" t="s">
         <v>43</v>
@@ -5744,7 +5790,7 @@
       <c r="F10" s="94"/>
       <c r="G10" s="94"/>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="95">
         <v>2</v>
       </c>
@@ -5757,7 +5803,7 @@
       <c r="F11" s="191"/>
       <c r="G11" s="96"/>
     </row>
-    <row r="12" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="97">
         <v>2.1</v>
       </c>
@@ -5776,7 +5822,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="85">
         <v>2.2000000000000002</v>
       </c>
@@ -5795,7 +5841,7 @@
       </c>
       <c r="G13" s="39"/>
     </row>
-    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="85">
         <v>2.2999999999999998</v>
       </c>
@@ -5814,7 +5860,7 @@
       </c>
       <c r="G14" s="40"/>
     </row>
-    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="85">
         <v>2.4</v>
       </c>
@@ -5833,7 +5879,7 @@
       </c>
       <c r="G15" s="41"/>
     </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="99">
         <v>2.5</v>
       </c>
@@ -5850,7 +5896,7 @@
       <c r="F16" s="102"/>
       <c r="G16" s="42"/>
     </row>
-    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="103"/>
       <c r="B17" s="90" t="s">
         <v>44</v>
@@ -5866,7 +5912,7 @@
       <c r="F17" s="94"/>
       <c r="G17" s="94"/>
     </row>
-    <row r="18" spans="1:8" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="105">
         <v>3</v>
       </c>
@@ -5879,7 +5925,7 @@
       <c r="F18" s="188"/>
       <c r="G18" s="106"/>
     </row>
-    <row r="19" spans="1:8" s="19" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="19" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="85">
         <v>3.1</v>
       </c>
@@ -5898,7 +5944,7 @@
       </c>
       <c r="G19" s="40"/>
     </row>
-    <row r="20" spans="1:8" s="20" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="20" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="107">
         <v>3.2</v>
       </c>
@@ -5919,7 +5965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="108">
         <v>3.3</v>
       </c>
@@ -5938,7 +5984,7 @@
       </c>
       <c r="G21" s="43"/>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="13" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="111"/>
       <c r="B22" s="90" t="s">
         <v>45</v>
@@ -5954,7 +6000,7 @@
       <c r="F22" s="115"/>
       <c r="G22" s="115"/>
     </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="116">
         <v>4</v>
       </c>
@@ -5968,7 +6014,7 @@
       <c r="G23" s="96"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="117">
         <v>4.0999999999999996</v>
       </c>
@@ -5988,7 +6034,7 @@
       <c r="G24" s="41"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" s="13" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="119">
         <v>4.2</v>
       </c>
@@ -6008,7 +6054,7 @@
       </c>
       <c r="G25" s="40"/>
     </row>
-    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="108">
         <v>4.3</v>
       </c>
@@ -6027,7 +6073,7 @@
       </c>
       <c r="G26" s="43"/>
     </row>
-    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="103"/>
       <c r="B27" s="90" t="s">
         <v>46</v>
@@ -6043,7 +6089,7 @@
       <c r="F27" s="123"/>
       <c r="G27" s="123"/>
     </row>
-    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="124"/>
       <c r="B28" s="125" t="s">
         <v>11</v>
@@ -6057,7 +6103,7 @@
       <c r="F28" s="127"/>
       <c r="G28" s="127"/>
     </row>
-    <row r="29" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="76">
         <v>5</v>
       </c>
@@ -6070,7 +6116,7 @@
       <c r="F29" s="188"/>
       <c r="G29" s="128"/>
     </row>
-    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="129"/>
       <c r="B30" s="130" t="s">
         <v>7</v>
@@ -6085,7 +6131,7 @@
       </c>
       <c r="G30" s="40"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="129"/>
       <c r="B31" s="130" t="s">
         <v>8</v>
@@ -6100,7 +6146,7 @@
       </c>
       <c r="G31" s="44"/>
     </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="111"/>
       <c r="B32" s="134" t="s">
         <v>49</v>
@@ -6115,7 +6161,7 @@
       </c>
       <c r="G32" s="45"/>
     </row>
-    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="137"/>
       <c r="B33" s="138" t="s">
         <v>55</v>
@@ -6128,7 +6174,7 @@
       <c r="F33" s="140"/>
       <c r="G33" s="140"/>
     </row>
-    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="141"/>
       <c r="B34" s="142" t="s">
         <v>31</v>
@@ -6142,7 +6188,7 @@
       <c r="F34" s="144"/>
       <c r="G34" s="145"/>
     </row>
-    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="12" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A35" s="33"/>
       <c r="B35" s="7"/>
       <c r="C35" s="21"/>
@@ -6151,7 +6197,7 @@
       <c r="F35" s="4"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A36" s="35"/>
       <c r="B36" s="9"/>
       <c r="C36" s="11"/>
@@ -6160,14 +6206,14 @@
       <c r="F36" s="10"/>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C38" s="18"/>
       <c r="D38" s="2"/>
       <c r="E38"/>
@@ -6175,7 +6221,6 @@
       <c r="G38"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -6203,69 +6248,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="115" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A5" s="64" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A7" s="64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A9" s="64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A11" s="64" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A12" s="64" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A13" s="146" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A14" s="146" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A15" s="146" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A17" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A18" s="64" t="s">
         <v>66</v>
       </c>
@@ -6277,25 +6322,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:B18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="67.85546875" style="46" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="67.86328125" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A6" s="50" t="s">
         <v>35</v>
       </c>
@@ -6303,10 +6348,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="49"/>
     </row>
-    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.35">
       <c r="A8" s="50" t="s">
         <v>34</v>
       </c>
@@ -6314,10 +6359,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="49"/>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A10" s="52" t="s">
         <v>36</v>
       </c>
@@ -6325,41 +6370,41 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A11" s="54"/>
       <c r="B11" s="55"/>
     </row>
-    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A12" s="56"/>
       <c r="B12" s="55" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="56"/>
       <c r="B13" s="57"/>
     </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A14" s="56"/>
       <c r="B14" s="55" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="56"/>
       <c r="B15" s="57"/>
     </row>
-    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A16" s="56"/>
       <c r="B16" s="60" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="56"/>
       <c r="B17" s="57"/>
     </row>
-    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.35">
       <c r="A18" s="58"/>
       <c r="B18" s="59" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
adds missing line in Bewertungsbogen
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen Projekte 5 und 6.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ProStudCreator\ProStudCreator\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA08397-D528-422D-92C5-BE605DFD560A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <definedName name="_Toc156968632" localSheetId="0">'1. Gesamtbewertung (Text)'!$A$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2. Detailbewertung (Excel)'!$A$1:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Samuel Vogel</author>
   </authors>
   <commentList>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -461,11 +460,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="37" x14ac:knownFonts="1">
     <font>
@@ -1327,10 +1326,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1355,17 +1354,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1375,7 +1374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1419,10 +1418,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -1496,7 +1491,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="17" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1584,7 +1579,7 @@
     <xf numFmtId="1" fontId="16" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1647,7 +1642,7 @@
     <xf numFmtId="1" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="18" fillId="3" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1745,9 +1740,51 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1787,48 +1824,6 @@
     <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1838,18 +1833,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="16" fillId="2" borderId="38" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="21" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="21" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1889,10 +1884,10 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1939,7 +1934,7 @@
         <xdr:cNvPr id="1054" name="Picture 3" descr="FHNW_HT_10mm">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2018,7 +2013,7 @@
         <xdr:cNvPr id="3" name="Textfeld 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2208,7 +2203,7 @@
         <xdr:cNvPr id="7" name="Textfeld 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2425,7 @@
         <xdr:cNvPr id="8" name="Textfeld 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2630,7 +2625,7 @@
         <xdr:cNvPr id="9" name="Textfeld 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2771,7 +2766,7 @@
         <xdr:cNvPr id="10" name="Textfeld 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2934,7 +2929,7 @@
         <xdr:cNvPr id="11" name="Textfeld 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3096,7 +3091,7 @@
         <xdr:cNvPr id="15" name="Textfeld 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3314,7 +3309,7 @@
         <xdr:cNvPr id="16" name="Textfeld 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3468,7 +3463,7 @@
         <xdr:cNvPr id="19" name="Textfeld 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3659,7 +3654,7 @@
         <xdr:cNvPr id="20" name="Textfeld 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3818,7 +3813,7 @@
         <xdr:cNvPr id="21" name="Textfeld 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3972,7 +3967,7 @@
         <xdr:cNvPr id="22" name="Textfeld 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4197,7 +4192,7 @@
         <xdr:cNvPr id="23" name="Textfeld 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4398,7 +4393,7 @@
         <xdr:cNvPr id="24" name="Textfeld 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4552,7 +4547,7 @@
         <xdr:cNvPr id="25" name="Textfeld 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4691,7 +4686,7 @@
         <xdr:cNvPr id="27" name="Textfeld 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4818,7 +4813,7 @@
         <xdr:cNvPr id="28" name="Textfeld 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4945,7 +4940,7 @@
         <xdr:cNvPr id="2" name="Textfeld 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5086,23 +5081,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5138,23 +5116,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5330,7 +5291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5340,271 +5301,265 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.265625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="80" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" style="2"/>
+    <col min="3" max="3" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="170"/>
-      <c r="C8" s="170"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+    </row>
+    <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="157"/>
+      <c r="C9" s="158"/>
+    </row>
+    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="173"/>
-      <c r="C10" s="174"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="159"/>
+      <c r="C10" s="160"/>
+    </row>
+    <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="170"/>
-      <c r="C11" s="170"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="156"/>
+      <c r="C11" s="156"/>
+    </row>
+    <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="170"/>
-      <c r="C12" s="170"/>
-    </row>
-    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="156"/>
+      <c r="C12" s="156"/>
+    </row>
+    <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="161" t="s">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="162"/>
-      <c r="C14" s="163"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="164"/>
-      <c r="B15" s="165"/>
-      <c r="C15" s="166"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="164"/>
-      <c r="B16" s="165"/>
-      <c r="C16" s="166"/>
-    </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="164"/>
-      <c r="B17" s="165"/>
-      <c r="C17" s="166"/>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="164"/>
-      <c r="B18" s="165"/>
-      <c r="C18" s="166"/>
-    </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="164"/>
-      <c r="B19" s="165"/>
-      <c r="C19" s="166"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="164"/>
-      <c r="B20" s="165"/>
-      <c r="C20" s="166"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="164"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="166"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="164"/>
-      <c r="B22" s="165"/>
-      <c r="C22" s="166"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="164"/>
-      <c r="B23" s="165"/>
-      <c r="C23" s="166"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="164"/>
-      <c r="B24" s="165"/>
-      <c r="C24" s="166"/>
-    </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="164"/>
-      <c r="B25" s="165"/>
-      <c r="C25" s="166"/>
-    </row>
-    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="164"/>
-      <c r="B26" s="165"/>
-      <c r="C26" s="166"/>
-    </row>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="164"/>
-      <c r="B27" s="165"/>
-      <c r="C27" s="166"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="164"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="164"/>
-      <c r="B29" s="165"/>
-      <c r="C29" s="166"/>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="164"/>
-      <c r="B30" s="165"/>
-      <c r="C30" s="166"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="164"/>
-      <c r="B31" s="165"/>
-      <c r="C31" s="166"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="164"/>
-      <c r="B32" s="165"/>
-      <c r="C32" s="166"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="164"/>
-      <c r="B33" s="165"/>
-      <c r="C33" s="166"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="164"/>
-      <c r="B34" s="165"/>
-      <c r="C34" s="166"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="167"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="169"/>
-    </row>
-    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="147"/>
+      <c r="C14" s="148"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="149"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="151"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="149"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="151"/>
+    </row>
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="149"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="151"/>
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="149"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="151"/>
+    </row>
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="149"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="151"/>
+    </row>
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="149"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="151"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="149"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="151"/>
+    </row>
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="149"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="151"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="149"/>
+      <c r="B23" s="150"/>
+      <c r="C23" s="151"/>
+    </row>
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="149"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="151"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="149"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="151"/>
+    </row>
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="149"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="151"/>
+    </row>
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="149"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="151"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="149"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="151"/>
+    </row>
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="149"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="151"/>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="149"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="151"/>
+    </row>
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="149"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="151"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="149"/>
+      <c r="B32" s="150"/>
+      <c r="C32" s="151"/>
+    </row>
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="149"/>
+      <c r="B33" s="150"/>
+      <c r="C33" s="151"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="149"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="151"/>
+    </row>
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="152"/>
+      <c r="B35" s="153"/>
+      <c r="C35" s="154"/>
+    </row>
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24"/>
       <c r="B36" s="25"/>
     </row>
-    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="147" t="s">
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="147"/>
+      <c r="B37" s="155"/>
       <c r="C37" s="31">
         <f>'2. Detailbewertung (Excel)'!C34</f>
         <v>4.2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="24"/>
       <c r="B38" s="25"/>
     </row>
-    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="147" t="s">
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="147"/>
-      <c r="C39" s="147"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="153" t="s">
+      <c r="B39" s="155"/>
+      <c r="C39" s="155"/>
+    </row>
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="154"/>
-      <c r="C40" s="155"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="156"/>
-      <c r="B41" s="157"/>
-      <c r="C41" s="158"/>
-    </row>
-    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="148" t="s">
+      <c r="B40" s="167"/>
+      <c r="C40" s="168"/>
+    </row>
+    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="169"/>
+      <c r="B41" s="170"/>
+      <c r="C41" s="171"/>
+    </row>
+    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="161" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="148"/>
-      <c r="C42" s="148"/>
-    </row>
-    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="161"/>
+      <c r="C42" s="161"/>
+    </row>
+    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24"/>
       <c r="B43" s="25"/>
     </row>
-    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="24"/>
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="159">
+      <c r="B45" s="172">
         <f ca="1">TODAY()</f>
-        <v>44459</v>
-      </c>
-      <c r="C45" s="160"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+        <v>44462</v>
+      </c>
+      <c r="C45" s="173"/>
+    </row>
+    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27"/>
-      <c r="B46" s="149"/>
-      <c r="C46" s="149"/>
-    </row>
-    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="162"/>
+      <c r="C46" s="162"/>
+    </row>
+    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="27"/>
-      <c r="B47" s="149"/>
-      <c r="C47" s="149"/>
-    </row>
-    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="162"/>
+      <c r="C47" s="162"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="149"/>
-      <c r="C48" s="149"/>
-    </row>
-    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="162"/>
+      <c r="C48" s="162"/>
+    </row>
+    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="28"/>
-      <c r="B49" s="149"/>
-      <c r="C49" s="149"/>
-    </row>
-    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="162"/>
+      <c r="C49" s="162"/>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="150"/>
-      <c r="C50" s="150"/>
-    </row>
-    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="163"/>
+      <c r="C50" s="163"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
-      <c r="B51" s="151"/>
-      <c r="C51" s="152"/>
+      <c r="B51" s="164"/>
+      <c r="C51" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A14:C35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C10"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
@@ -5615,6 +5570,12 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5625,570 +5586,570 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="34" customWidth="1"/>
-    <col min="2" max="2" width="45.86328125" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.86328125" customWidth="1"/>
-    <col min="6" max="6" width="65.86328125" customWidth="1"/>
-    <col min="7" max="7" width="66.73046875" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" customWidth="1"/>
+    <col min="7" max="7" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="37" customFormat="1" ht="29.65" x14ac:dyDescent="0.65">
-      <c r="A1" s="65"/>
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="1:7" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-    </row>
-    <row r="2" spans="1:7" s="37" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-    </row>
-    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69"/>
-      <c r="B3" s="175" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+    </row>
+    <row r="2" spans="1:7" s="37" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+    </row>
+    <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="68"/>
+      <c r="B3" s="174" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-    </row>
-    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="69"/>
-      <c r="B4" s="176" t="s">
+      <c r="C3" s="174"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+    </row>
+    <row r="4" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68"/>
+      <c r="B4" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-    </row>
-    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71" t="s">
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="176"/>
+    </row>
+    <row r="5" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="69"/>
+      <c r="B5" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75" t="s">
+      <c r="E5" s="73"/>
+      <c r="F5" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="74" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="76">
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="75">
         <v>1</v>
       </c>
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="185" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="188"/>
-      <c r="G6" s="77"/>
-    </row>
-    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="78">
+      <c r="C6" s="186"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="76"/>
+    </row>
+    <row r="7" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="77">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="62">
         <v>2</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="61">
         <v>4</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81" t="s">
+      <c r="E7" s="79"/>
+      <c r="F7" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="40"/>
-    </row>
-    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="82">
+      <c r="G7" s="39"/>
+    </row>
+    <row r="8" spans="1:7" ht="206.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="81">
         <v>1.2</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="60">
         <v>1</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="61">
         <v>4</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="E8" s="79"/>
+      <c r="F8" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="40"/>
-    </row>
-    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="85">
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="1:7" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="84">
         <v>1.3</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="62">
         <v>1</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="61">
         <v>4</v>
       </c>
-      <c r="E9" s="88"/>
-      <c r="F9" s="81" t="s">
+      <c r="E9" s="87"/>
+      <c r="F9" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="89"/>
-      <c r="B10" s="90" t="s">
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="88"/>
+      <c r="B10" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="91">
+      <c r="C10" s="90">
         <v>1</v>
       </c>
-      <c r="D10" s="92">
+      <c r="D10" s="91">
         <f>(C7*D7+C8*D8+C9*D9)/SUM(C7:C9)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="93"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="95">
+      <c r="E10" s="92"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="94">
         <v>2</v>
       </c>
-      <c r="B11" s="189" t="s">
+      <c r="B11" s="188" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="190"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="190"/>
-      <c r="F11" s="191"/>
-      <c r="G11" s="96"/>
-    </row>
-    <row r="12" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="97">
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="190"/>
+      <c r="G11" s="95"/>
+    </row>
+    <row r="12" spans="1:7" ht="165.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="96">
         <v>2.1</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="62">
         <v>2</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="61">
         <v>4</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81" t="s">
+      <c r="E12" s="79"/>
+      <c r="F12" s="80" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="85">
+    <row r="13" spans="1:7" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="84">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="87">
+      <c r="C13" s="86">
+        <v>2</v>
+      </c>
+      <c r="D13" s="61">
+        <v>4</v>
+      </c>
+      <c r="E13" s="87"/>
+      <c r="F13" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="84">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="86">
         <v>1</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D14" s="61">
         <v>4</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="81" t="s">
+      <c r="E14" s="87"/>
+      <c r="F14" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="39"/>
-    </row>
-    <row r="14" spans="1:7" ht="205.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="85">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B14" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="87">
-        <v>2</v>
-      </c>
-      <c r="D14" s="62">
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="84">
+        <v>2.4</v>
+      </c>
+      <c r="B15" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="88"/>
-      <c r="F14" s="81" t="s">
+      <c r="C15" s="86">
+        <v>1</v>
+      </c>
+      <c r="D15" s="61">
+        <v>4</v>
+      </c>
+      <c r="E15" s="87"/>
+      <c r="F15" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="40"/>
-    </row>
-    <row r="15" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="85">
-        <v>2.4</v>
-      </c>
-      <c r="B15" s="86" t="s">
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="98">
+        <v>2.5</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="86">
+        <v>1</v>
+      </c>
+      <c r="D16" s="61">
         <v>4</v>
       </c>
-      <c r="C15" s="87">
-        <v>1</v>
-      </c>
-      <c r="D15" s="62">
+      <c r="E16" s="100"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="102"/>
+      <c r="B17" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="103">
         <v>4</v>
       </c>
-      <c r="E15" s="88"/>
-      <c r="F15" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="41"/>
-    </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" ht="205.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99">
-        <v>2.5</v>
-      </c>
-      <c r="B16" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="87">
-        <v>1</v>
-      </c>
-      <c r="D16" s="62">
-        <v>4</v>
-      </c>
-      <c r="E16" s="101"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="42"/>
-    </row>
-    <row r="17" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="103"/>
-      <c r="B17" s="90" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="104">
-        <v>4</v>
-      </c>
-      <c r="D17" s="92">
+      <c r="D17" s="91">
         <f>(C12*D12+C13*D13+C14*D14+C15*D15+C16*D16)/SUM(C12:C16)</f>
         <v>4</v>
       </c>
-      <c r="E17" s="93"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-    </row>
-    <row r="18" spans="1:8" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="105">
+      <c r="E17" s="92"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+    </row>
+    <row r="18" spans="1:8" s="36" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="104">
         <v>3</v>
       </c>
-      <c r="B18" s="186" t="s">
+      <c r="B18" s="185" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="192"/>
-      <c r="D18" s="192"/>
-      <c r="E18" s="187"/>
-      <c r="F18" s="188"/>
-      <c r="G18" s="106"/>
-    </row>
-    <row r="19" spans="1:8" s="19" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="85">
+      <c r="C18" s="191"/>
+      <c r="D18" s="191"/>
+      <c r="E18" s="186"/>
+      <c r="F18" s="187"/>
+      <c r="G18" s="105"/>
+    </row>
+    <row r="19" spans="1:8" s="19" customFormat="1" ht="180.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="84">
         <v>3.1</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="87">
+      <c r="C19" s="86">
         <v>1</v>
       </c>
-      <c r="D19" s="62">
+      <c r="D19" s="61">
         <v>4</v>
       </c>
-      <c r="E19" s="80"/>
-      <c r="F19" s="81" t="s">
+      <c r="E19" s="79"/>
+      <c r="F19" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="40"/>
-    </row>
-    <row r="20" spans="1:8" s="20" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="107">
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:8" s="20" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="106">
         <v>3.2</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="87">
+      <c r="C20" s="86">
         <v>1</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="61">
         <v>4</v>
       </c>
-      <c r="E20" s="88"/>
-      <c r="F20" s="81" t="s">
+      <c r="E20" s="87"/>
+      <c r="F20" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G20" s="39" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="108">
+    <row r="21" spans="1:8" ht="192.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="107">
         <v>3.3</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="87">
+      <c r="C21" s="86">
         <v>1</v>
       </c>
-      <c r="D21" s="62">
+      <c r="D21" s="61">
         <v>4</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="81" t="s">
+      <c r="E21" s="109"/>
+      <c r="F21" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="43"/>
-    </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="111"/>
-      <c r="B22" s="90" t="s">
+      <c r="G21" s="42"/>
+    </row>
+    <row r="22" spans="1:8" s="13" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="110"/>
+      <c r="B22" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="112">
+      <c r="C22" s="111">
         <v>2</v>
       </c>
-      <c r="D22" s="113">
+      <c r="D22" s="112">
         <f>(C19*D19+C20*D20+C21*D21)/SUM(C19:C21)</f>
         <v>4</v>
       </c>
-      <c r="E22" s="114"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="116">
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="114"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="115">
         <v>4</v>
       </c>
-      <c r="B23" s="186" t="s">
+      <c r="B23" s="185" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="192"/>
-      <c r="D23" s="192"/>
-      <c r="E23" s="187"/>
-      <c r="F23" s="188"/>
-      <c r="G23" s="96"/>
+      <c r="C23" s="191"/>
+      <c r="D23" s="191"/>
+      <c r="E23" s="186"/>
+      <c r="F23" s="187"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="117">
+    <row r="24" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="116">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="61">
+      <c r="C24" s="60">
         <v>1</v>
       </c>
-      <c r="D24" s="62">
+      <c r="D24" s="61">
         <v>4</v>
       </c>
-      <c r="E24" s="118"/>
-      <c r="F24" s="81" t="s">
+      <c r="E24" s="117"/>
+      <c r="F24" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="41"/>
+      <c r="G24" s="40"/>
       <c r="H24" s="17"/>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="119">
+    <row r="25" spans="1:8" s="13" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="118">
         <v>4.2</v>
       </c>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="84">
+      <c r="C25" s="83">
         <f>2-C24</f>
         <v>1</v>
       </c>
-      <c r="D25" s="62">
+      <c r="D25" s="61">
         <v>4</v>
       </c>
-      <c r="E25" s="120"/>
-      <c r="F25" s="81" t="s">
+      <c r="E25" s="119"/>
+      <c r="F25" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="40"/>
-    </row>
-    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="108">
+      <c r="G25" s="39"/>
+    </row>
+    <row r="26" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="107">
         <v>4.3</v>
       </c>
-      <c r="B26" s="121" t="s">
+      <c r="B26" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="84">
+      <c r="C26" s="83">
         <v>1</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="61">
         <v>4</v>
       </c>
-      <c r="E26" s="110"/>
-      <c r="F26" s="81" t="s">
+      <c r="E26" s="109"/>
+      <c r="F26" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="43"/>
-    </row>
-    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="103"/>
-      <c r="B27" s="90" t="s">
+      <c r="G26" s="42"/>
+    </row>
+    <row r="27" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="102"/>
+      <c r="B27" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="112">
+      <c r="C27" s="111">
         <v>1</v>
       </c>
-      <c r="D27" s="113">
+      <c r="D27" s="112">
         <f>(C24*D24+C25*D25+C26*D26)/SUM(C24:C26)</f>
         <v>4</v>
       </c>
-      <c r="E27" s="122"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-    </row>
-    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="124"/>
-      <c r="B28" s="125" t="s">
+      <c r="E27" s="121"/>
+      <c r="F27" s="122"/>
+      <c r="G27" s="122"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="123"/>
+      <c r="B28" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="193">
+      <c r="C28" s="192">
         <f>(C10*D10+C17*D17+C22*D22+C27*D27)/SUM(C10,C17,C22,C27)</f>
         <v>4</v>
       </c>
-      <c r="D28" s="194"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="127"/>
-    </row>
-    <row r="29" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="76">
+      <c r="D28" s="193"/>
+      <c r="E28" s="125"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+    </row>
+    <row r="29" spans="1:8" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="75">
         <v>5</v>
       </c>
-      <c r="B29" s="186" t="s">
+      <c r="B29" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="187"/>
-      <c r="D29" s="187"/>
-      <c r="E29" s="187"/>
-      <c r="F29" s="188"/>
-      <c r="G29" s="128"/>
-    </row>
-    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="129"/>
-      <c r="B30" s="130" t="s">
+      <c r="C29" s="186"/>
+      <c r="D29" s="186"/>
+      <c r="E29" s="186"/>
+      <c r="F29" s="187"/>
+      <c r="G29" s="127"/>
+    </row>
+    <row r="30" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="128"/>
+      <c r="B30" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="182">
+      <c r="C30" s="181">
         <v>5</v>
       </c>
-      <c r="D30" s="183"/>
-      <c r="E30" s="131"/>
-      <c r="F30" s="132" t="s">
+      <c r="D30" s="182"/>
+      <c r="E30" s="130"/>
+      <c r="F30" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="40"/>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="129"/>
-      <c r="B31" s="130" t="s">
+      <c r="G30" s="39"/>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="128"/>
+      <c r="B31" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="182">
+      <c r="C31" s="181">
         <v>0</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="133"/>
-      <c r="F31" s="132" t="s">
+      <c r="D31" s="182"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="44"/>
-    </row>
-    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="111"/>
-      <c r="B32" s="134" t="s">
+      <c r="G31" s="43"/>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="110"/>
+      <c r="B32" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="184">
+      <c r="C32" s="183">
         <v>5</v>
       </c>
-      <c r="D32" s="185"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="136" t="s">
+      <c r="D32" s="184"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="45"/>
-    </row>
-    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="137"/>
-      <c r="B33" s="138" t="s">
+      <c r="G32" s="44"/>
+    </row>
+    <row r="33" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="136"/>
+      <c r="B33" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="178">
+      <c r="C33" s="177">
         <v>0.2</v>
       </c>
-      <c r="D33" s="179"/>
-      <c r="E33" s="139"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-    </row>
-    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="141"/>
-      <c r="B34" s="142" t="s">
+      <c r="D33" s="178"/>
+      <c r="E33" s="138"/>
+      <c r="F33" s="139"/>
+      <c r="G33" s="139"/>
+    </row>
+    <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="140"/>
+      <c r="B34" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="180">
+      <c r="C34" s="179">
         <f>ROUND(C28+C33,1)</f>
         <v>4.2</v>
       </c>
-      <c r="D34" s="181"/>
-      <c r="E34" s="143"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="145"/>
-    </row>
-    <row r="35" spans="1:7" s="12" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="D34" s="180"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="143"/>
+      <c r="G34" s="144"/>
+    </row>
+    <row r="35" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="33"/>
       <c r="B35" s="7"/>
       <c r="C35" s="21"/>
@@ -6197,7 +6158,7 @@
       <c r="F35" s="4"/>
       <c r="G35"/>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="35"/>
       <c r="B36" s="9"/>
       <c r="C36" s="11"/>
@@ -6206,14 +6167,14 @@
       <c r="F36" s="10"/>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C38" s="18"/>
       <c r="D38" s="2"/>
       <c r="E38"/>
@@ -6248,70 +6209,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="115" style="48" customWidth="1"/>
+    <col min="1" max="1" width="115" style="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="64" t="s">
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="64" t="s">
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="64" t="s">
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="64" t="s">
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="146" t="s">
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="145" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="146" t="s">
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="145" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="146" t="s">
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="145" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="64" t="s">
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="63" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="64" t="s">
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="63" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6322,91 +6283,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.265625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="67.86328125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="49"/>
-    </row>
-    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.35">
-      <c r="A8" s="50" t="s">
+    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="48"/>
+    </row>
+    <row r="8" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="49"/>
-    </row>
-    <row r="10" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="48"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-      <c r="B11" s="55"/>
-    </row>
-    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
-      <c r="B12" s="55" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
+    </row>
+    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="55"/>
+      <c r="B12" s="54" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-    </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
-      <c r="B14" s="55" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+    </row>
+    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="55"/>
+      <c r="B14" s="54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
-      <c r="B15" s="57"/>
-    </row>
-    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="60" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+    </row>
+    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="55"/>
+      <c r="B16" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="56"/>
-      <c r="B17" s="57"/>
-    </row>
-    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.35">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+    </row>
+    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="57"/>
+      <c r="B18" s="58" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>